<commit_message>
Added IC data of pw after incubation.
</commit_message>
<xml_diff>
--- a/index/data/Seq_extr_data.xlsx
+++ b/index/data/Seq_extr_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Documents\studie\scriptie\Master\Master_Thesis\index\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB70F550-8250-47C5-AA76-D9F0129CFBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72FEB1F1-42AE-4AEB-9F2A-6A0426F3E0D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -570,42 +570,7 @@
     <cellStyle name="Normal 2" xfId="2" xr:uid="{B84C7E2D-E01B-4520-A8F6-532897D289E4}"/>
     <cellStyle name="Normal 3" xfId="1" xr:uid="{4C0C0E25-6857-48AB-82D3-B6E341AC7F6D}"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <color theme="0" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -883,8 +848,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Y26" sqref="Y26"/>
+    <sheetView tabSelected="1" topLeftCell="E82" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2:Q116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1032,13 +997,13 @@
         <v>607.22799999999995</v>
       </c>
       <c r="O2">
-        <v>11.846982849883551</v>
+        <v>11.129023774684999</v>
       </c>
       <c r="P2">
         <v>6.3774931187804382</v>
       </c>
       <c r="Q2">
-        <v>5.4694897311031125</v>
+        <v>4.7515306559045607</v>
       </c>
       <c r="R2" s="8">
         <v>181.70963829489801</v>
@@ -1106,13 +1071,13 @@
         <v>790.96299999999997</v>
       </c>
       <c r="O3">
-        <v>19.225280542028379</v>
+        <v>13.617782253788063</v>
       </c>
       <c r="P3">
         <v>10.021956383654461</v>
       </c>
       <c r="Q3">
-        <v>9.2033241583739187</v>
+        <v>3.5958258701336021</v>
       </c>
       <c r="R3" s="8">
         <v>233.620002601506</v>
@@ -1180,13 +1145,13 @@
         <v>771.73099999999999</v>
       </c>
       <c r="O4">
-        <v>18.302985390641552</v>
+        <v>12.710096804260875</v>
       </c>
       <c r="P4">
         <v>12.464641117933519</v>
       </c>
       <c r="Q4">
-        <v>5.8383442727080332</v>
+        <v>0.24545568632735559</v>
       </c>
       <c r="R4" s="8">
         <v>206.69453062501</v>
@@ -1254,13 +1219,13 @@
         <v>667.69</v>
       </c>
       <c r="O5">
-        <v>13.103260639424096</v>
+        <v>12.36540137941976</v>
       </c>
       <c r="P5">
         <v>7.8336015244547967</v>
       </c>
       <c r="Q5">
-        <v>5.2696591149692997</v>
+        <v>4.5317998549649632</v>
       </c>
       <c r="R5" s="8">
         <v>172.320181356539</v>
@@ -1328,13 +1293,13 @@
         <v>1399.4069999999999</v>
       </c>
       <c r="O6">
-        <v>30.726021596442948</v>
+        <v>24.936344753195264</v>
       </c>
       <c r="P6">
         <v>13.883019267414781</v>
       </c>
       <c r="Q6">
-        <v>16.843002329028167</v>
+        <v>11.053325485780483</v>
       </c>
       <c r="R6" s="8">
         <v>384.01767117848499</v>
@@ -1402,13 +1367,13 @@
         <v>1513.3789999999999</v>
       </c>
       <c r="O7">
-        <v>32.724327757781083</v>
+        <v>26.89799553874369</v>
       </c>
       <c r="P7">
         <v>7.2131484226127478</v>
       </c>
       <c r="Q7">
-        <v>25.511179335168336</v>
+        <v>19.684847116130943</v>
       </c>
       <c r="R7" s="8">
         <v>428.685169081808</v>
@@ -1476,13 +1441,13 @@
         <v>566.82399999999996</v>
       </c>
       <c r="O8">
-        <v>11.083993224645356</v>
+        <v>10.378120357348873</v>
       </c>
       <c r="P8">
         <v>6.9797798009739598</v>
       </c>
       <c r="Q8">
-        <v>4.1042134236713963</v>
+        <v>3.3983405563749134</v>
       </c>
       <c r="R8" s="8">
         <v>160.64423592966401</v>
@@ -1550,13 +1515,13 @@
         <v>220.399</v>
       </c>
       <c r="O9">
-        <v>4.3702625449925909</v>
+        <v>4.0358870734796684</v>
       </c>
       <c r="P9">
         <v>5.3128202413720098</v>
       </c>
       <c r="Q9">
-        <v>-0.94255769637941889</v>
+        <v>-1.2769331678923415</v>
       </c>
       <c r="R9" s="8">
         <v>51.526539322829201</v>
@@ -1624,13 +1589,13 @@
         <v>206.61799999999999</v>
       </c>
       <c r="O10">
-        <v>3.9559284353165372</v>
+        <v>3.6281162616844993</v>
       </c>
       <c r="P10">
         <v>5.1618992165996209</v>
       </c>
       <c r="Q10">
-        <v>-1.2059707812830838</v>
+        <v>-1.5337829549151216</v>
       </c>
       <c r="R10" s="8">
         <v>49.173116275429699</v>
@@ -1698,13 +1663,13 @@
         <v>196.56399999999999</v>
       </c>
       <c r="O11">
-        <v>3.8776730891382609</v>
+        <v>3.5511005265731019</v>
       </c>
       <c r="P11">
         <v>4.9641647258098685</v>
       </c>
       <c r="Q11">
-        <v>-1.0864916366716075</v>
+        <v>-1.4130641992367665</v>
       </c>
       <c r="R11" s="8">
         <v>54.574695296654298</v>
@@ -1772,13 +1737,13 @@
         <v>190.55799999999999</v>
       </c>
       <c r="O12">
-        <v>3.4933834427270809</v>
+        <v>3.1728982559367731</v>
       </c>
       <c r="P12">
         <v>4.7370844802032623</v>
       </c>
       <c r="Q12">
-        <v>-1.2437010374761814</v>
+        <v>-1.5641862242664892</v>
       </c>
       <c r="R12" s="8">
         <v>46.854791089660402</v>
@@ -1846,13 +1811,13 @@
         <v>188.69800000000001</v>
       </c>
       <c r="O13">
-        <v>3.9391594325640487</v>
+        <v>3.6116128898749142</v>
       </c>
       <c r="P13">
         <v>4.6064260004234612</v>
       </c>
       <c r="Q13">
-        <v>-0.66726656785941252</v>
+        <v>-0.99481311054854693</v>
       </c>
       <c r="R13" s="8">
         <v>44.520209522147802</v>
@@ -1920,13 +1885,13 @@
         <v>101.773</v>
       </c>
       <c r="O14">
-        <v>2.101556214270591</v>
+        <v>1.8031183957411994</v>
       </c>
       <c r="P14">
         <v>3.3361740419225079</v>
       </c>
       <c r="Q14">
-        <v>-1.2346178276519169</v>
+        <v>-1.5330556461813085</v>
       </c>
       <c r="R14" s="8">
         <v>23.293854949443801</v>
@@ -1994,13 +1959,13 @@
         <v>54.652000000000001</v>
       </c>
       <c r="O15">
-        <v>1.0762587338556004</v>
+        <v>1.0061805730998488</v>
       </c>
       <c r="P15">
         <v>0.97243065847977994</v>
       </c>
       <c r="Q15">
-        <v>0.10382807537582051</v>
+        <v>3.3749914620068822E-2</v>
       </c>
       <c r="R15" s="8">
         <v>21.316504369081201</v>
@@ -2068,13 +2033,13 @@
         <v>31.134</v>
       </c>
       <c r="O16">
-        <v>0.63425576963794217</v>
+        <v>0.57117919781886473</v>
       </c>
       <c r="P16">
         <v>0.63635189498200317</v>
       </c>
       <c r="Q16">
-        <v>-2.0961253440610061E-3</v>
+        <v>-6.5172697163138449E-2</v>
       </c>
       <c r="R16" s="8">
         <v>14.1452474313491</v>
@@ -2142,13 +2107,13 @@
         <v>27.385000000000002</v>
       </c>
       <c r="O17">
-        <v>0.55264662290916811</v>
+        <v>0.49086278834554997</v>
       </c>
       <c r="P17">
         <v>0.52763286047004032</v>
       </c>
       <c r="Q17">
-        <v>2.5013762439127785E-2</v>
+        <v>-3.6770072124490349E-2</v>
       </c>
       <c r="R17" s="8">
         <v>15.882745546651901</v>
@@ -2216,13 +2181,13 @@
         <v>12.788</v>
       </c>
       <c r="O18">
-        <v>0.27917213635401239</v>
+        <v>0.22172029975089744</v>
       </c>
       <c r="P18">
         <v>0.26002752487825548</v>
       </c>
       <c r="Q18">
-        <v>1.9144611475756912E-2</v>
+        <v>-3.8307225127358041E-2</v>
       </c>
       <c r="R18" s="8">
         <v>13.0343368180044</v>
@@ -2290,13 +2255,13 @@
         <v>4.0620000000000003</v>
       </c>
       <c r="O19">
-        <v>0.11455642600042354</v>
+        <v>5.9712199820135703E-2</v>
       </c>
       <c r="P19">
         <v>0.10547321617615932</v>
       </c>
       <c r="Q19">
-        <v>9.0832098242642212E-3</v>
+        <v>-4.5761016356023615E-2</v>
       </c>
       <c r="R19" s="8">
         <v>3.4188054960937002</v>
@@ -2364,13 +2329,13 @@
         <v>83.858000000000004</v>
       </c>
       <c r="O20">
-        <v>1.7724645352530179</v>
+        <v>1.4792397239780892</v>
       </c>
       <c r="P20">
         <v>8.1272178699978834</v>
       </c>
       <c r="Q20">
-        <v>-6.3547533347448653</v>
+        <v>-6.6479781460197938</v>
       </c>
       <c r="R20" s="8">
         <v>22.434036644283399</v>
@@ -2438,13 +2403,13 @@
         <v>81.644000000000005</v>
       </c>
       <c r="O21">
-        <v>1.7682722845648957</v>
+        <v>1.4751138810256923</v>
       </c>
       <c r="P21">
         <v>7.4354965064577598</v>
       </c>
       <c r="Q21">
-        <v>-5.6672242218928641</v>
+        <v>-5.960382625432068</v>
       </c>
       <c r="R21" s="8">
         <v>20.9608336498783</v>
@@ -2512,13 +2477,13 @@
         <v>93.399000000000001</v>
       </c>
       <c r="O22">
-        <v>1.918494600889266</v>
+        <v>1.6229565868198936</v>
       </c>
       <c r="P22">
         <v>5.685930552614864</v>
       </c>
       <c r="Q22">
-        <v>-3.7674359517255978</v>
+        <v>-4.0629739657949706</v>
       </c>
       <c r="R22" s="8">
         <v>24.2562372232982</v>
@@ -2586,13 +2551,13 @@
         <v>74.507000000000005</v>
       </c>
       <c r="O23">
-        <v>1.5838132542875296</v>
+        <v>1.2935767911202549</v>
       </c>
       <c r="P23">
         <v>5.6335274190133404</v>
       </c>
       <c r="Q23">
-        <v>-4.0497141647258106</v>
+        <v>-4.3399506278930851</v>
       </c>
       <c r="R23" s="8">
         <v>20.738050486065401</v>
@@ -2660,13 +2625,13 @@
         <v>50.003</v>
       </c>
       <c r="O24">
-        <v>0.95258733855600264</v>
+        <v>0.88446820600415776</v>
       </c>
       <c r="P24">
         <v>0.93945161973322067</v>
       </c>
       <c r="Q24">
-        <v>1.3135718822781972E-2</v>
+        <v>-5.4983413729062902E-2</v>
       </c>
       <c r="R24" s="8">
         <v>15.423879092557099</v>
@@ -2734,13 +2699,13 @@
         <v>47.384999999999998</v>
       </c>
       <c r="O25">
-        <v>0.94029006987084507</v>
+        <v>0.8723657333437953</v>
       </c>
       <c r="P25">
         <v>0.88914461147575707</v>
       </c>
       <c r="Q25">
-        <v>5.1145458395087995E-2</v>
+        <v>-1.6778878131961772E-2</v>
       </c>
       <c r="R25" s="8">
         <v>16.6167382375186</v>
@@ -2808,13 +2773,13 @@
         <v>30.15</v>
       </c>
       <c r="O26">
-        <v>0.61315477450772837</v>
+        <v>0.55041245495847002</v>
       </c>
       <c r="P26">
         <v>0.56997459242007209</v>
       </c>
       <c r="Q26">
-        <v>4.3180182087656283E-2</v>
+        <v>-1.9562137461602069E-2</v>
       </c>
       <c r="R26" s="8">
         <v>14.2982450197473</v>
@@ -2882,13 +2847,13 @@
         <v>19.172000000000001</v>
       </c>
       <c r="O27">
-        <v>0.4066165572729199</v>
+        <v>0.34714592550374523</v>
       </c>
       <c r="P27">
         <v>0.36832733432140602</v>
       </c>
       <c r="Q27">
-        <v>3.8289222951513879E-2</v>
+        <v>-2.1181408817660785E-2</v>
       </c>
       <c r="R27" s="8">
         <v>11.288238363564099</v>
@@ -2956,13 +2921,13 @@
         <v>21.861999999999998</v>
       </c>
       <c r="O28">
-        <v>0.45049544780859635</v>
+        <v>0.39032974840549328</v>
       </c>
       <c r="P28">
         <v>0.413184416684311</v>
       </c>
       <c r="Q28">
-        <v>3.7311031124285354E-2</v>
+        <v>-2.2854668278817714E-2</v>
       </c>
       <c r="R28" s="8">
         <v>14.4103788716764</v>
@@ -3030,13 +2995,13 @@
         <v>15.872999999999999</v>
       </c>
       <c r="O29">
-        <v>0.33618674571247109</v>
+        <v>0.27783176390348729</v>
       </c>
       <c r="P29">
         <v>0.31494600889265301</v>
       </c>
       <c r="Q29">
-        <v>2.1240736819818085E-2</v>
+        <v>-3.7114244989165712E-2</v>
       </c>
       <c r="R29" s="8">
         <v>13.8702007965831</v>
@@ -3104,13 +3069,13 @@
         <v>11.965999999999999</v>
       </c>
       <c r="O30">
-        <v>0.26142494177429615</v>
+        <v>0.20425423125241973</v>
       </c>
       <c r="P30">
         <v>0.24898793139953429</v>
       </c>
       <c r="Q30">
-        <v>1.2437010374761859E-2</v>
+        <v>-4.4733700147114558E-2</v>
       </c>
       <c r="R30" s="8">
         <v>9.6195661129406709</v>
@@ -3178,13 +3143,13 @@
         <v>10.654999999999999</v>
       </c>
       <c r="O31">
-        <v>0.23585221257675215</v>
+        <v>0.17908658924280221</v>
       </c>
       <c r="P31">
         <v>0.22327546051238631</v>
       </c>
       <c r="Q31">
-        <v>1.2576752064365843E-2</v>
+        <v>-4.4188871269584096E-2</v>
       </c>
       <c r="R31" s="8">
         <v>9.4065208134830591</v>
@@ -3252,13 +3217,13 @@
         <v>13.689</v>
       </c>
       <c r="O32">
-        <v>0.30055261486343438</v>
+        <v>0.24276209880811858</v>
       </c>
       <c r="P32">
         <v>0.27344272708024575</v>
       </c>
       <c r="Q32">
-        <v>2.7109887783188624E-2</v>
+        <v>-3.0680628272127169E-2</v>
       </c>
       <c r="R32" s="8">
         <v>12.762419356565299</v>
@@ -3326,13 +3291,13 @@
         <v>7.0519999999999996</v>
       </c>
       <c r="O33">
-        <v>0.16989413508363338</v>
+        <v>0.11417332679176699</v>
       </c>
       <c r="P33">
         <v>0.15605970781283093</v>
       </c>
       <c r="Q33">
-        <v>1.3834427270802446E-2</v>
+        <v>-4.1886381021063943E-2</v>
       </c>
       <c r="R33" s="8">
         <v>9.2985161265469198</v>
@@ -3400,13 +3365,13 @@
         <v>6.2069999999999999</v>
       </c>
       <c r="O34">
-        <v>0.15508151598560246</v>
+        <v>9.9595348359966696E-2</v>
       </c>
       <c r="P34">
         <v>0.14278424730044473</v>
       </c>
       <c r="Q34">
-        <v>1.2297268685157736E-2</v>
+        <v>-4.3188898940478032E-2</v>
       </c>
       <c r="R34" s="8">
         <v>7.6333743265517304</v>
@@ -3474,13 +3439,13 @@
         <v>14.956</v>
       </c>
       <c r="O35">
-        <v>0.31802032606394259</v>
+        <v>0.25995311110976993</v>
       </c>
       <c r="P35">
         <v>0.30460512386195226</v>
       </c>
       <c r="Q35">
-        <v>1.3415202201990328E-2</v>
+        <v>-4.4652012752182335E-2</v>
       </c>
       <c r="R35" s="8">
         <v>14.3616316991343</v>
@@ -3548,13 +3513,13 @@
         <v>5.7460000000000004</v>
       </c>
       <c r="O36">
-        <v>0.14571882278213008</v>
+        <v>9.0380965766281587E-2</v>
       </c>
       <c r="P36">
         <v>0.13146517044251543</v>
       </c>
       <c r="Q36">
-        <v>1.4253652339614648E-2</v>
+        <v>-4.1084204676233846E-2</v>
       </c>
       <c r="R36" s="8">
         <v>8.8165700549639308</v>
@@ -3622,13 +3587,13 @@
         <v>364.80200000000002</v>
       </c>
       <c r="O37">
-        <v>9.1165572729197599</v>
+        <v>6.3206663775271341</v>
       </c>
       <c r="P37">
         <v>5.9067224221892873</v>
       </c>
       <c r="Q37">
-        <v>3.2098348507304726</v>
+        <v>0.41394395533784678</v>
       </c>
       <c r="R37" s="8">
         <v>104.244227905245</v>
@@ -3696,13 +3661,13 @@
         <v>507.84</v>
       </c>
       <c r="O38">
-        <v>9.9898157950455229</v>
+        <v>9.3012753467734353</v>
       </c>
       <c r="P38">
         <v>6.9392547109887799</v>
       </c>
       <c r="Q38">
-        <v>3.050561084056743</v>
+        <v>2.3620206357846554</v>
       </c>
       <c r="R38" s="8">
         <v>136.21303323980999</v>
@@ -3770,13 +3735,13 @@
         <v>790.37300000000005</v>
       </c>
       <c r="O39">
-        <v>19.378996400592857</v>
+        <v>13.769063162042594</v>
       </c>
       <c r="P39">
         <v>6.8484226127461367</v>
       </c>
       <c r="Q39">
-        <v>12.53057378784672</v>
+        <v>6.9206405492964569</v>
       </c>
       <c r="R39" s="8">
         <v>250.480641069554</v>
@@ -3844,13 +3809,13 @@
         <v>728.02099999999996</v>
       </c>
       <c r="O40">
-        <v>16.376138047850947</v>
+        <v>13.465251090093409</v>
       </c>
       <c r="P40">
         <v>3.1335485919966133</v>
       </c>
       <c r="Q40">
-        <v>13.242589455854334</v>
+        <v>10.331702498096796</v>
       </c>
       <c r="R40" s="8">
         <v>237.16743946282099</v>
@@ -3918,13 +3883,13 @@
         <v>579.72699999999998</v>
       </c>
       <c r="O41">
-        <v>13.308807961041715</v>
+        <v>10.446509329923444</v>
       </c>
       <c r="P41">
         <v>11.638926529748044</v>
       </c>
       <c r="Q41">
-        <v>1.6698814312936712</v>
+        <v>-1.1924171998246003</v>
       </c>
       <c r="R41" s="8">
         <v>172.88134835296</v>
@@ -3992,13 +3957,13 @@
         <v>741.81600000000003</v>
       </c>
       <c r="O42">
-        <v>18.372856235443585</v>
+        <v>12.77886085346748</v>
       </c>
       <c r="P42">
         <v>7.1404827440186338</v>
       </c>
       <c r="Q42">
-        <v>11.232373491424951</v>
+        <v>5.6383781094488459</v>
       </c>
       <c r="R42" s="8">
         <v>248.68654213957799</v>
@@ -4066,13 +4031,13 @@
         <v>1008.107</v>
       </c>
       <c r="O43">
-        <v>23.585221257675219</v>
+        <v>17.908658924280221</v>
       </c>
       <c r="P43">
         <v>9.0577387253864092</v>
       </c>
       <c r="Q43">
-        <v>14.527482532288809</v>
+        <v>8.850920198893812</v>
       </c>
       <c r="R43" s="8">
         <v>345.27266213621198</v>
@@ -4140,13 +4105,13 @@
         <v>1547.3710000000001</v>
       </c>
       <c r="O44">
-        <v>34.205589667584178</v>
+        <v>28.360794403684206</v>
       </c>
       <c r="P44">
         <v>5.6438492483590963</v>
       </c>
       <c r="Q44">
-        <v>28.561740419225082</v>
+        <v>22.71694515532511</v>
       </c>
       <c r="R44" s="8">
         <v>504.61576466511798</v>
@@ -4214,13 +4179,13 @@
         <v>936.59100000000001</v>
       </c>
       <c r="O45">
-        <v>19.953525301715018</v>
+        <v>16.985970409471591</v>
       </c>
       <c r="P45">
         <v>3.2173936057590522</v>
       </c>
       <c r="Q45">
-        <v>16.736131695955965</v>
+        <v>13.768576803712538</v>
       </c>
       <c r="R45" s="8">
         <v>261.57474303496201</v>
@@ -4288,13 +4253,13 @@
         <v>531.55700000000002</v>
       </c>
       <c r="O46">
-        <v>10.436989201778532</v>
+        <v>9.7413652616957087</v>
       </c>
       <c r="P46">
         <v>6.4445691297903895</v>
       </c>
       <c r="Q46">
-        <v>3.9924200719881426</v>
+        <v>3.2967961319053192</v>
       </c>
       <c r="R46" s="8">
         <v>149.064253132837</v>
@@ -4362,13 +4327,13 @@
         <v>181.703</v>
       </c>
       <c r="O47">
-        <v>3.5842155409697236</v>
+        <v>3.2622915199053599</v>
       </c>
       <c r="P47">
         <v>3.6652657209400812</v>
       </c>
       <c r="Q47">
-        <v>-8.1050179970357572E-2</v>
+        <v>-0.40297420103472126</v>
       </c>
       <c r="R47" s="8">
         <v>53.265507367550398</v>
@@ -4436,13 +4401,13 @@
         <v>132.017</v>
       </c>
       <c r="O48">
-        <v>2.7429705695532514</v>
+        <v>2.4343723674578346</v>
       </c>
       <c r="P48">
         <v>3.1363434257886946</v>
       </c>
       <c r="Q48">
-        <v>-0.39337285623544327</v>
+        <v>-0.70197105833086004</v>
       </c>
       <c r="R48" s="8">
         <v>37.315104637493398</v>
@@ -4510,13 +4475,13 @@
         <v>77.295000000000002</v>
       </c>
       <c r="O49">
-        <v>1.6299280118568711</v>
+        <v>1.3389610635966145</v>
       </c>
       <c r="P49">
         <v>2.3859305526148642</v>
       </c>
       <c r="Q49">
-        <v>-0.75600254075799311</v>
+        <v>-1.0469694890182497</v>
       </c>
       <c r="R49" s="8">
         <v>27.489945265577401</v>
@@ -4584,13 +4549,13 @@
         <v>62.098999999999997</v>
       </c>
       <c r="O50">
-        <v>1.2231272496294729</v>
+        <v>1.1507226045321328</v>
       </c>
       <c r="P50">
         <v>1.197834003811137</v>
       </c>
       <c r="Q50">
-        <v>2.5293245818335919E-2</v>
+        <v>-4.7111399279004207E-2</v>
       </c>
       <c r="R50" s="8">
         <v>32.128920173833002</v>
@@ -4658,13 +4623,13 @@
         <v>44.575000000000003</v>
       </c>
       <c r="O51">
-        <v>0.87069870844802055</v>
+        <v>0.80387674033401657</v>
       </c>
       <c r="P51">
         <v>0.84330933728562374</v>
       </c>
       <c r="Q51">
-        <v>2.7389371162396814E-2</v>
+        <v>-3.9432596951607168E-2</v>
       </c>
       <c r="R51" s="8">
         <v>28.233213142977998</v>
@@ -4732,13 +4697,13 @@
         <v>26.141999999999999</v>
       </c>
       <c r="O52">
-        <v>0.52791234384924846</v>
+        <v>0.46652031492641172</v>
       </c>
       <c r="P52">
         <v>0.51743171712894365</v>
       </c>
       <c r="Q52">
-        <v>1.0480626720304809E-2</v>
+        <v>-5.091140220253193E-2</v>
       </c>
       <c r="R52" s="8">
         <v>23.2392000549975</v>
@@ -4806,13 +4771,13 @@
         <v>20.823</v>
       </c>
       <c r="O53">
-        <v>0.43093161126402724</v>
+        <v>0.37107581462764377</v>
       </c>
       <c r="P53">
         <v>0.42492271861105246</v>
       </c>
       <c r="Q53">
-        <v>6.0088926529747733E-3</v>
+        <v>-5.3846903983408689E-2</v>
       </c>
       <c r="R53" s="8">
         <v>24.801329817442099</v>
@@ -4880,13 +4845,13 @@
         <v>8.3160000000000007</v>
       </c>
       <c r="O54">
-        <v>0.19378996400592857</v>
+        <v>0.13769063162042597</v>
       </c>
       <c r="P54">
         <v>0.18400804573364396</v>
       </c>
       <c r="Q54">
-        <v>9.7819182722846121E-3</v>
+        <v>-4.6317414113217992E-2</v>
       </c>
       <c r="R54" s="8">
         <v>11.5251794356445</v>
@@ -4954,13 +4919,13 @@
         <v>81.984999999999999</v>
       </c>
       <c r="O55">
-        <v>1.7214588185475341</v>
+        <v>1.429041968057267</v>
       </c>
       <c r="P55">
         <v>3.1125873385560037</v>
       </c>
       <c r="Q55">
-        <v>-1.3911285200084695</v>
+        <v>-1.6835453704987366</v>
       </c>
       <c r="R55" s="8">
         <v>29.229079951753398</v>
@@ -5028,13 +4993,13 @@
         <v>49.779000000000003</v>
       </c>
       <c r="O56">
-        <v>0.96111158162185073</v>
+        <v>0.89285742000736357</v>
       </c>
       <c r="P56">
         <v>0.91611475756934169</v>
       </c>
       <c r="Q56">
-        <v>4.4996824052509043E-2</v>
+        <v>-2.325733756197812E-2</v>
       </c>
       <c r="R56" s="8">
         <v>17.147963050864899</v>
@@ -5102,13 +5067,13 @@
         <v>55.234000000000002</v>
       </c>
       <c r="O57">
-        <v>1.113849248359094</v>
+        <v>1.0431756315730025</v>
       </c>
       <c r="P57">
         <v>1.0547385136565746</v>
       </c>
       <c r="Q57">
-        <v>5.9110734702519485E-2</v>
+        <v>-1.1562882083572035E-2</v>
       </c>
       <c r="R57" s="8">
         <v>21.6256085859902</v>
@@ -5176,13 +5141,13 @@
         <v>44.554000000000002</v>
       </c>
       <c r="O58">
-        <v>0.86972051662079219</v>
+        <v>0.80291404364512409</v>
       </c>
       <c r="P58">
         <v>0.82975439339402945</v>
       </c>
       <c r="Q58">
-        <v>3.996612322676274E-2</v>
+        <v>-2.6840349748905368E-2</v>
       </c>
       <c r="R58" s="8">
         <v>18.371625455044899</v>
@@ -5250,13 +5215,13 @@
         <v>48.218000000000004</v>
       </c>
       <c r="O59">
-        <v>0.95482320558966771</v>
+        <v>0.88666865557876917</v>
       </c>
       <c r="P59">
         <v>0.89599195426635625</v>
       </c>
       <c r="Q59">
-        <v>5.8831251323311462E-2</v>
+        <v>-9.3232986875870782E-3</v>
       </c>
       <c r="R59" s="8">
         <v>22.334933710011398</v>
@@ -5324,13 +5289,13 @@
         <v>46.313000000000002</v>
       </c>
       <c r="O60">
-        <v>0.92729409273766694</v>
+        <v>0.85957562019136657</v>
       </c>
       <c r="P60">
         <v>0.89040228668219368</v>
       </c>
       <c r="Q60">
-        <v>3.6891806055473264E-2</v>
+        <v>-3.0826666490827104E-2</v>
       </c>
       <c r="R60" s="8">
         <v>21.806979102198301</v>
@@ -5398,13 +5363,13 @@
         <v>36.802</v>
       </c>
       <c r="O61">
-        <v>0.73766461994495047</v>
+        <v>0.67294999064464034</v>
       </c>
       <c r="P61">
         <v>0.7164238831251325</v>
       </c>
       <c r="Q61">
-        <v>2.1240736819817974E-2</v>
+        <v>-4.347389248049216E-2</v>
       </c>
       <c r="R61" s="8">
         <v>16.189289206780799</v>
@@ -5472,13 +5437,13 @@
         <v>52.076000000000001</v>
       </c>
       <c r="O62">
-        <v>1.0156108405674362</v>
+        <v>0.94649337838851566</v>
       </c>
       <c r="P62">
         <v>1.0051302138471314</v>
       </c>
       <c r="Q62">
-        <v>1.0480626720304809E-2</v>
+        <v>-5.8636835458615755E-2</v>
       </c>
       <c r="R62" s="8">
         <v>18.704471050625099</v>
@@ -5546,13 +5511,13 @@
         <v>60.219000000000001</v>
       </c>
       <c r="O63">
-        <v>1.1490641541393185</v>
+        <v>1.0778327123731315</v>
       </c>
       <c r="P63">
         <v>1.1826021596442942</v>
       </c>
       <c r="Q63">
-        <v>-3.3538005504975654E-2</v>
+        <v>-0.10476944727116266</v>
       </c>
       <c r="R63" s="8">
         <v>22.065810202962201</v>
@@ -5620,13 +5585,13 @@
         <v>45.26</v>
       </c>
       <c r="O64">
-        <v>0.8941753123015036</v>
+        <v>0.82698146086743585</v>
       </c>
       <c r="P64">
         <v>0.77958712682617004</v>
       </c>
       <c r="Q64">
-        <v>0.11458818547533356</v>
+        <v>4.7394334041265807E-2</v>
       </c>
       <c r="R64" s="8">
         <v>20.965656443263399</v>
@@ -5694,13 +5659,13 @@
         <v>55.045999999999999</v>
       </c>
       <c r="O65">
-        <v>1.0748613169595598</v>
+        <v>1.0048052921157167</v>
       </c>
       <c r="P65">
         <v>0.99744442091890761</v>
       </c>
       <c r="Q65">
-        <v>7.7416896040652161E-2</v>
+        <v>7.3608711968090601E-3</v>
       </c>
       <c r="R65" s="8">
         <v>23.3239987243382</v>
@@ -5768,13 +5733,13 @@
         <v>46.929000000000002</v>
       </c>
       <c r="O66">
-        <v>0.91108405674359538</v>
+        <v>0.84362236077543451</v>
       </c>
       <c r="P66">
         <v>0.89165996188863028</v>
       </c>
       <c r="Q66">
-        <v>1.9424094854965102E-2</v>
+        <v>-4.8037601113195771E-2</v>
       </c>
       <c r="R66" s="8">
         <v>23.4544685532945</v>
@@ -5842,13 +5807,13 @@
         <v>27.844000000000001</v>
       </c>
       <c r="O67">
-        <v>0.55069023925471117</v>
+        <v>0.488937394967765</v>
       </c>
       <c r="P67">
         <v>0.52958924412449726</v>
       </c>
       <c r="Q67">
-        <v>2.1100995130213906E-2</v>
+        <v>-4.0651849156732256E-2</v>
       </c>
       <c r="R67" s="8">
         <v>16.0170163761127</v>
@@ -5916,13 +5881,13 @@
         <v>22.965</v>
       </c>
       <c r="O68">
-        <v>0.47439127673089154</v>
+        <v>0.41384705323415222</v>
       </c>
       <c r="P68">
         <v>0.45818124073681998</v>
       </c>
       <c r="Q68">
-        <v>1.6210035994071559E-2</v>
+        <v>-4.4334187502667766E-2</v>
       </c>
       <c r="R68" s="8">
         <v>10.391549548137201</v>
@@ -5990,13 +5955,13 @@
         <v>19.064</v>
       </c>
       <c r="O69">
-        <v>0.39012703789964021</v>
+        <v>0.3309176098909864</v>
       </c>
       <c r="P69">
         <v>0.38481685369468571</v>
       </c>
       <c r="Q69">
-        <v>5.3101842049544934E-3</v>
+        <v>-5.3899243803699315E-2</v>
       </c>
       <c r="R69" s="8">
         <v>9.69572536593307</v>
@@ -6064,13 +6029,13 @@
         <v>11.99</v>
       </c>
       <c r="O70">
-        <v>0.26463900063518964</v>
+        <v>0.20741737751592357</v>
       </c>
       <c r="P70">
         <v>0.25206224857082371</v>
       </c>
       <c r="Q70">
-        <v>1.2576752064365926E-2</v>
+        <v>-4.4644871054900143E-2</v>
       </c>
       <c r="R70" s="8">
         <v>8.5683298219971693</v>
@@ -6138,13 +6103,13 @@
         <v>15.387</v>
       </c>
       <c r="O71">
-        <v>0.32542663561295798</v>
+        <v>0.26724210032567003</v>
       </c>
       <c r="P71">
         <v>0.31592420071988159</v>
       </c>
       <c r="Q71">
-        <v>9.5024348930763947E-3</v>
+        <v>-4.8682100394211558E-2</v>
       </c>
       <c r="R71" s="8">
         <v>10.803048704969401</v>
@@ -6212,13 +6177,13 @@
         <v>12.976000000000001</v>
       </c>
       <c r="O72">
-        <v>0.28252593690450994</v>
+        <v>0.22502097411281449</v>
       </c>
       <c r="P72">
         <v>0.28252593690450994</v>
       </c>
       <c r="Q72">
-        <v>0</v>
+        <v>-5.7504962791695452E-2</v>
       </c>
       <c r="R72" s="8">
         <v>11.4123605693313</v>
@@ -6286,13 +6251,13 @@
         <v>10.773999999999999</v>
       </c>
       <c r="O73">
-        <v>0.2401842049544782</v>
+        <v>0.18334996029361175</v>
       </c>
       <c r="P73">
         <v>0.23780859623120909</v>
       </c>
       <c r="Q73">
-        <v>2.3756087232691125E-3</v>
+        <v>-5.4458635937597338E-2</v>
       </c>
       <c r="R73" s="8">
         <v>9.6548974655843605</v>
@@ -6360,13 +6325,13 @@
         <v>5.2329999999999997</v>
       </c>
       <c r="O74">
-        <v>0.13649587126826179</v>
+        <v>8.1304111271009713E-2</v>
       </c>
       <c r="P74">
         <v>0.12210247723904306</v>
       </c>
       <c r="Q74">
-        <v>1.4393394029218728E-2</v>
+        <v>-4.0798365968033351E-2</v>
       </c>
       <c r="R74" s="8">
         <v>7.75223828534864</v>
@@ -6434,13 +6399,13 @@
         <v>424.77800000000002</v>
       </c>
       <c r="O75">
-        <v>8.5127461359305538</v>
+        <v>7.847603346545803</v>
       </c>
       <c r="P75">
         <v>6.0714588185475353</v>
       </c>
       <c r="Q75">
-        <v>2.4412873173830185</v>
+        <v>1.7761445279982677</v>
       </c>
       <c r="R75" s="8">
         <v>116.51937623951299</v>
@@ -6508,13 +6473,13 @@
         <v>946.47699999999998</v>
       </c>
       <c r="O76">
-        <v>22.299597713317819</v>
+        <v>16.643400418878688</v>
       </c>
       <c r="P76">
         <v>9.0381748888418407</v>
       </c>
       <c r="Q76">
-        <v>13.261422824475979</v>
+        <v>7.6052255300368472</v>
       </c>
       <c r="R76" s="8">
         <v>265.782912941392</v>
@@ -6582,13 +6547,13 @@
         <v>637.00300000000004</v>
       </c>
       <c r="O77">
-        <v>12.369616769002754</v>
+        <v>11.643378862750405</v>
       </c>
       <c r="P77">
         <v>6.1706754181664207</v>
       </c>
       <c r="Q77">
-        <v>6.1989413508363329</v>
+        <v>5.4727034445839839</v>
       </c>
       <c r="R77" s="8">
         <v>169.711052545141</v>
@@ -6656,13 +6621,13 @@
         <v>672.46199999999999</v>
       </c>
       <c r="O78">
-        <v>13.150772813889482</v>
+        <v>12.412160932880253</v>
       </c>
       <c r="P78">
         <v>6.158098666102056</v>
       </c>
       <c r="Q78">
-        <v>6.9926741477874259</v>
+        <v>6.2540622667781971</v>
       </c>
       <c r="R78" s="8">
         <v>180.42980003184601</v>
@@ -6730,13 +6695,13 @@
         <v>347.87099999999998</v>
       </c>
       <c r="O79">
-        <v>8.8580351471522381</v>
+        <v>6.066239395462695</v>
       </c>
       <c r="P79">
         <v>5.9067224221892873</v>
       </c>
       <c r="Q79">
-        <v>2.9513127249629507</v>
+        <v>0.15951697327340764</v>
       </c>
       <c r="R79" s="8">
         <v>87.725017009253804</v>
@@ -6804,13 +6769,13 @@
         <v>202.73599999999999</v>
       </c>
       <c r="O80">
-        <v>4.0076328604700411</v>
+        <v>3.6790016580973872</v>
       </c>
       <c r="P80">
         <v>5.0619839085327127</v>
       </c>
       <c r="Q80">
-        <v>-1.0543510480626717</v>
+        <v>-1.3829822504353255</v>
       </c>
       <c r="R80" s="8">
         <v>39.882330638931201</v>
@@ -6878,13 +6843,13 @@
         <v>103.16</v>
       </c>
       <c r="O81">
-        <v>2.1239148846072418</v>
+        <v>1.8251228914873125</v>
       </c>
       <c r="P81">
         <v>3.369712047427484</v>
       </c>
       <c r="Q81">
-        <v>-1.2457971628202422</v>
+        <v>-1.5445891559401714</v>
       </c>
       <c r="R81" s="8">
         <v>17.9833393889006</v>
@@ -6952,13 +6917,13 @@
         <v>89.725999999999999</v>
       </c>
       <c r="O82">
-        <v>1.9059178488249</v>
+        <v>1.6105790579627044</v>
       </c>
       <c r="P82">
         <v>3.1335485919966133</v>
       </c>
       <c r="Q82">
-        <v>-1.2276307431717133</v>
+        <v>-1.5229695340339089</v>
       </c>
       <c r="R82" s="8">
         <v>20.699565537531701</v>
@@ -7026,13 +6991,13 @@
         <v>69.197999999999993</v>
       </c>
       <c r="O83">
-        <v>1.3407897522760961</v>
+        <v>1.2665212633960559</v>
       </c>
       <c r="P83">
         <v>1.2350052932458186</v>
       </c>
       <c r="Q83">
-        <v>0.10578445903027744</v>
+        <v>3.1515970150237216E-2</v>
       </c>
       <c r="R83" s="8">
         <v>16.941509205644099</v>
@@ -7100,13 +7065,13 @@
         <v>63.899000000000001</v>
       </c>
       <c r="O84">
-        <v>1.2513550709294941</v>
+        <v>1.1785032804116014</v>
       </c>
       <c r="P84">
         <v>1.1342515350412876</v>
       </c>
       <c r="Q84">
-        <v>0.11710353588820643</v>
+        <v>4.4251745370313733E-2</v>
       </c>
       <c r="R84" s="8">
         <v>17.597408244740102</v>
@@ -7174,13 +7139,13 @@
         <v>53.158000000000001</v>
       </c>
       <c r="O85">
-        <v>1.0621448232055897</v>
+        <v>0.99229023516011461</v>
       </c>
       <c r="P85">
         <v>1.059908956171925</v>
       </c>
       <c r="Q85">
-        <v>2.2358670336646291E-3</v>
+        <v>-6.7618721011810434E-2</v>
       </c>
       <c r="R85" s="8">
         <v>14.341002390939</v>
@@ -7248,13 +7213,13 @@
         <v>31.916</v>
       </c>
       <c r="O86">
-        <v>0.63160067753546489</v>
+        <v>0.56856616394901371</v>
       </c>
       <c r="P86">
         <v>0.6366313783612112</v>
       </c>
       <c r="Q86">
-        <v>-5.0307008257463037E-3</v>
+        <v>-6.8065214412197483E-2</v>
       </c>
       <c r="R86" s="8">
         <v>11.4974136891983</v>
@@ -7322,13 +7287,13 @@
         <v>36.317</v>
       </c>
       <c r="O87">
-        <v>0.73486978615286913</v>
+        <v>0.67019942867637616</v>
       </c>
       <c r="P87">
         <v>0.73850307008257488</v>
       </c>
       <c r="Q87">
-        <v>-3.633283929705744E-3</v>
+        <v>-6.8303641406198712E-2</v>
       </c>
       <c r="R87" s="8">
         <v>12.6212657361909</v>
@@ -7396,13 +7361,13 @@
         <v>40.122999999999998</v>
       </c>
       <c r="O88">
-        <v>0.79481897099301302</v>
+        <v>0.72919898289564333</v>
       </c>
       <c r="P88">
         <v>0.7801460935845862</v>
       </c>
       <c r="Q88">
-        <v>1.4672877408426821E-2</v>
+        <v>-5.0947110688942865E-2</v>
       </c>
       <c r="R88" s="8">
         <v>14.1344925078893</v>
@@ -7470,13 +7435,13 @@
         <v>30.727</v>
       </c>
       <c r="O89">
-        <v>0.61119839085327143</v>
+        <v>0.54848706158068505</v>
       </c>
       <c r="P89">
         <v>0.60169595596019498</v>
       </c>
       <c r="Q89">
-        <v>9.5024348930764502E-3</v>
+        <v>-5.320889437950993E-2</v>
       </c>
       <c r="R89" s="8">
         <v>14.244720784632101</v>
@@ -7544,13 +7509,13 @@
         <v>16.015000000000001</v>
       </c>
       <c r="O90">
-        <v>0.34373279695109049</v>
+        <v>0.28525828121780056</v>
       </c>
       <c r="P90">
         <v>0.33730467922930352</v>
       </c>
       <c r="Q90">
-        <v>6.4281177217869745E-3</v>
+        <v>-5.2046398011502959E-2</v>
       </c>
       <c r="R90" s="8">
         <v>9.9861824487404593</v>
@@ -7618,13 +7583,13 @@
         <v>17.672999999999998</v>
       </c>
       <c r="O91">
-        <v>0.37112216811348731</v>
+        <v>0.31221378850678982</v>
       </c>
       <c r="P91">
         <v>0.34624814736396375</v>
       </c>
       <c r="Q91">
-        <v>2.4874020749523551E-2</v>
+        <v>-3.403435885717393E-2</v>
       </c>
       <c r="R91" s="8">
         <v>12.278190927974</v>
@@ -7692,13 +7657,13 @@
         <v>12.965</v>
       </c>
       <c r="O92">
-        <v>0.28001058649163679</v>
+        <v>0.2225454683413767</v>
       </c>
       <c r="P92">
         <v>0.27651704425153517</v>
       </c>
       <c r="Q92">
-        <v>3.4935422401016214E-3</v>
+        <v>-5.397157591015847E-2</v>
       </c>
       <c r="R92" s="8">
         <v>9.6147416327355195</v>
@@ -7766,13 +7731,13 @@
         <v>17.539000000000001</v>
       </c>
       <c r="O93">
-        <v>0.36567224221892869</v>
+        <v>0.30685019266867453</v>
       </c>
       <c r="P93">
         <v>0.36134024984120278</v>
       </c>
       <c r="Q93">
-        <v>4.3319923777259128E-3</v>
+        <v>-5.449005717252825E-2</v>
       </c>
       <c r="R93" s="8">
         <v>11.861851963998699</v>
@@ -7840,13 +7805,13 @@
         <v>17.106000000000002</v>
       </c>
       <c r="O94">
-        <v>0.36692991742536535</v>
+        <v>0.30808794555439351</v>
       </c>
       <c r="P94">
         <v>0.36078128308278645</v>
       </c>
       <c r="Q94">
-        <v>6.1486343425788959E-3</v>
+        <v>-5.2693337528392947E-2</v>
       </c>
       <c r="R94" s="8">
         <v>11.3837250990897</v>
@@ -7914,13 +7879,13 @@
         <v>18.117000000000001</v>
       </c>
       <c r="O95">
-        <v>0.38286047004022877</v>
+        <v>0.32376614877349946</v>
       </c>
       <c r="P95">
         <v>0.37782976921448247</v>
       </c>
       <c r="Q95">
-        <v>5.0307008257463037E-3</v>
+        <v>-5.4063620440983007E-2</v>
       </c>
       <c r="R95" s="8">
         <v>11.8651767112987</v>
@@ -7988,13 +7953,13 @@
         <v>612.76599999999996</v>
       </c>
       <c r="O96">
-        <v>12.220093161126407</v>
+        <v>11.496223797448271</v>
       </c>
       <c r="P96">
         <v>11.617806478932884</v>
       </c>
       <c r="Q96">
-        <v>0.60228668219352244</v>
+        <v>-0.12158268148461282</v>
       </c>
       <c r="R96" s="8">
         <v>150.17016907611</v>
@@ -8062,13 +8027,13 @@
         <v>892.09400000000005</v>
       </c>
       <c r="O97">
-        <v>20.343214058860905</v>
+        <v>14.718007041093744</v>
       </c>
       <c r="P97">
         <v>9.1234173195003212</v>
       </c>
       <c r="Q97">
-        <v>11.219796739360584</v>
+        <v>5.5945897215934224</v>
       </c>
       <c r="R97" s="8">
         <v>253.01611318504999</v>
@@ -8136,13 +8101,13 @@
         <v>394.73200000000003</v>
       </c>
       <c r="O98">
-        <v>7.9146517044251548</v>
+        <v>7.2589830853372641</v>
       </c>
       <c r="P98">
         <v>6.9616133813254297</v>
       </c>
       <c r="Q98">
-        <v>0.95303832309972503</v>
+        <v>0.29736970401183438</v>
       </c>
       <c r="R98" s="8">
         <v>88.452012288605303</v>
@@ -8210,13 +8175,13 @@
         <v>231.80199999999999</v>
       </c>
       <c r="O99">
-        <v>4.6155092102477244</v>
+        <v>4.2772488861948519</v>
       </c>
       <c r="P99">
         <v>5.9053250052932471</v>
       </c>
       <c r="Q99">
-        <v>-1.2898157950455227</v>
+        <v>-1.6280761190983952</v>
       </c>
       <c r="R99" s="8">
         <v>47.232846722437301</v>
@@ -8284,13 +8249,13 @@
         <v>98.234999999999999</v>
       </c>
       <c r="O100">
-        <v>2.0058331568918066</v>
+        <v>1.7089116483281501</v>
       </c>
       <c r="P100">
         <v>3.2173936057590522</v>
       </c>
       <c r="Q100">
-        <v>-1.2115604488672456</v>
+        <v>-1.5084819574309021</v>
       </c>
       <c r="R100" s="8">
         <v>18.0234287910537</v>
@@ -8358,13 +8323,13 @@
         <v>16.023</v>
       </c>
       <c r="O101">
-        <v>0.33716493753969945</v>
+        <v>0.27879446059237967</v>
       </c>
       <c r="P101">
         <v>0.32193309337285636</v>
       </c>
       <c r="Q101">
-        <v>1.5231844166843089E-2</v>
+        <v>-4.3138632780476693E-2</v>
       </c>
       <c r="R101" s="8">
         <v>11.0736253740856</v>
@@ -8432,13 +8397,13 @@
         <v>77.549000000000007</v>
       </c>
       <c r="O102">
-        <v>1.6599724751217455</v>
+        <v>1.3685296047554545</v>
       </c>
       <c r="P102">
         <v>2.9071670548380277</v>
       </c>
       <c r="Q102">
-        <v>-1.2471945797162822</v>
+        <v>-1.5386374500825732</v>
       </c>
       <c r="R102" s="8">
         <v>14.846062104767</v>
@@ -8506,13 +8471,13 @@
         <v>119.428</v>
       </c>
       <c r="O103">
-        <v>2.4613910650010595</v>
+        <v>2.1572532491552154</v>
       </c>
       <c r="P103">
         <v>3.6652657209400812</v>
       </c>
       <c r="Q103">
-        <v>-1.2038746559390217</v>
+        <v>-1.5080124717848657</v>
       </c>
       <c r="R103" s="8">
         <v>19.989594206322</v>
@@ -8580,13 +8545,13 @@
         <v>90.418000000000006</v>
       </c>
       <c r="O104">
-        <v>1.8926423883125139</v>
+        <v>1.5975138886134499</v>
       </c>
       <c r="P104">
         <v>3.1363434257886946</v>
       </c>
       <c r="Q104">
-        <v>-1.2437010374761808</v>
+        <v>-1.5388295371752447</v>
       </c>
       <c r="R104" s="8">
         <v>15.2686986477059</v>
@@ -8654,13 +8619,13 @@
         <v>79.225999999999999</v>
       </c>
       <c r="O105">
-        <v>4.7510586491636682</v>
+        <v>4.4106511416556664</v>
       </c>
       <c r="P105">
         <v>2.3859305526148642</v>
       </c>
       <c r="Q105">
-        <v>2.365128096548804</v>
+        <v>2.0247205890408022</v>
       </c>
       <c r="R105" s="8">
         <v>13.769811610994701</v>
@@ -8728,13 +8693,13 @@
         <v>47.56</v>
       </c>
       <c r="O106">
-        <v>1.9574634766038543</v>
+        <v>1.3961602499821089</v>
       </c>
       <c r="P106">
         <v>0.92994918484014422</v>
       </c>
       <c r="Q106">
-        <v>1.0275142917637101</v>
+        <v>0.46621106514196464</v>
       </c>
       <c r="R106" s="8">
         <v>9.6520983821587496</v>
@@ -8802,13 +8767,13 @@
         <v>58.908999999999999</v>
       </c>
       <c r="O107">
-        <v>1.143753969934364</v>
+        <v>1.0726066446334295</v>
       </c>
       <c r="P107">
         <v>1.0759792504763923</v>
       </c>
       <c r="Q107">
-        <v>6.7774719457971644E-2</v>
+        <v>-3.3726058429628392E-3</v>
       </c>
       <c r="R107" s="8">
         <v>16.776701184818599</v>
@@ -8876,13 +8841,13 @@
         <v>50.780999999999999</v>
       </c>
       <c r="O108">
-        <v>0.99241372009316142</v>
+        <v>0.92366371405192271</v>
       </c>
       <c r="P108">
         <v>0.93302350201143347</v>
       </c>
       <c r="Q108">
-        <v>5.9390218081727952E-2</v>
+        <v>-9.3597879595107569E-3</v>
       </c>
       <c r="R108" s="8">
         <v>15.799263583929299</v>
@@ -8950,13 +8915,13 @@
         <v>54.197000000000003</v>
       </c>
       <c r="O109">
-        <v>1.0716472580986662</v>
+        <v>1.0016421458522129</v>
       </c>
       <c r="P109">
         <v>0.97466652551344513</v>
       </c>
       <c r="Q109">
-        <v>9.6980732585221108E-2</v>
+        <v>2.697562033876777E-2</v>
       </c>
       <c r="R109" s="8">
         <v>19.0315210966458</v>
@@ -9024,13 +8989,13 @@
         <v>51.491</v>
       </c>
       <c r="O110">
-        <v>1.0086237560872329</v>
+        <v>0.93961697346785511</v>
       </c>
       <c r="P110">
         <v>0.94965276307431734</v>
       </c>
       <c r="Q110">
-        <v>5.8970993012915529E-2</v>
+        <v>-1.0035789606462231E-2</v>
       </c>
       <c r="R110" s="8">
         <v>19.5568882243441</v>
@@ -9098,13 +9063,13 @@
         <v>38.231999999999999</v>
       </c>
       <c r="O111">
-        <v>0.75471310607664643</v>
+        <v>0.68972841865105206</v>
       </c>
       <c r="P111">
         <v>0.70133178064789348</v>
       </c>
       <c r="Q111">
-        <v>5.3381325428752957E-2</v>
+        <v>-1.1603361996841421E-2</v>
       </c>
       <c r="R111" s="8">
         <v>14.5473220746997</v>
@@ -9172,13 +9137,13 @@
         <v>40.104999999999997</v>
       </c>
       <c r="O112">
-        <v>0.79286258733855619</v>
+        <v>0.72727358951785848</v>
       </c>
       <c r="P112">
         <v>0.75457336438704237</v>
       </c>
       <c r="Q112">
-        <v>3.8289222951513824E-2</v>
+        <v>-2.729977486918389E-2</v>
       </c>
       <c r="R112" s="8">
         <v>17.497162968359898</v>
@@ -9246,13 +9211,13 @@
         <v>36.923000000000002</v>
       </c>
       <c r="O113">
-        <v>0.74101842049544786</v>
+        <v>0.67625066500655751</v>
       </c>
       <c r="P113">
         <v>0.69769849671818784</v>
       </c>
       <c r="Q113">
-        <v>4.3319923777260017E-2</v>
+        <v>-2.1447831711630339E-2</v>
       </c>
       <c r="R113" s="8">
         <v>15.631093814280501</v>
@@ -9320,13 +9285,13 @@
         <v>34.183</v>
       </c>
       <c r="O114">
-        <v>0.67030912555579103</v>
+        <v>0.6066614472094729</v>
       </c>
       <c r="P114">
         <v>0.63104171077704863</v>
       </c>
       <c r="Q114">
-        <v>3.9267414778742404E-2</v>
+        <v>-2.4380263567575722E-2</v>
       </c>
       <c r="R114" s="8">
         <v>15.403222066042799</v>
@@ -9394,13 +9359,13 @@
         <v>33.735999999999997</v>
       </c>
       <c r="O115">
-        <v>0.6560554732161763</v>
+        <v>0.5926335811713257</v>
       </c>
       <c r="P115">
         <v>0.63579292822358691</v>
       </c>
       <c r="Q115">
-        <v>2.0262544992589393E-2</v>
+        <v>-4.315934705226121E-2</v>
       </c>
       <c r="R115" s="8">
         <v>15.226071474371601</v>
@@ -9468,13 +9433,13 @@
         <v>30.5</v>
       </c>
       <c r="O116">
-        <v>0.62237772602159669</v>
+        <v>0.55948930945374187</v>
       </c>
       <c r="P116">
         <v>0.60001905568494629</v>
       </c>
       <c r="Q116">
-        <v>2.2358670336650399E-2</v>
+        <v>-4.0529746231204422E-2</v>
       </c>
       <c r="R116" s="8">
         <v>14.274239814948899</v>

</xml_diff>

<commit_message>
Created sequential extraction script, added new ICP data and made nice figures.
</commit_message>
<xml_diff>
--- a/index/data/Seq_extr_data.xlsx
+++ b/index/data/Seq_extr_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harmv\Documents\studie\scriptie\Master\Master_Thesis\index\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEF2984-7892-46A9-8BF3-FE47996C0A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2163EC4-16AA-4C0B-A9B3-ED320883E0DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -855,8 +855,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="V25" sqref="V25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,10 +998,10 @@
         <v>14.8939</v>
       </c>
       <c r="L2">
-        <v>-4.2530000000000001</v>
+        <v>6.3419999999999996</v>
       </c>
       <c r="M2">
-        <v>-0.98699999999999999</v>
+        <v>4.7030000000000003</v>
       </c>
       <c r="N2">
         <v>152.297</v>
@@ -1025,10 +1025,10 @@
         <v>10.127000000000001</v>
       </c>
       <c r="U2">
-        <v>0.108</v>
+        <v>0.04</v>
       </c>
       <c r="V2">
-        <v>7.0000000000000007E-2</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="W2">
         <v>25.95</v>
@@ -1075,10 +1075,10 @@
         <v>15.1502</v>
       </c>
       <c r="L3">
-        <v>-9.9860000000000007</v>
+        <v>2.1360000000000001</v>
       </c>
       <c r="M3">
-        <v>-9.8109999999999999</v>
+        <v>1.996</v>
       </c>
       <c r="N3">
         <v>139.744</v>
@@ -1102,10 +1102,10 @@
         <v>17.75</v>
       </c>
       <c r="U3">
-        <v>-6.3E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="V3">
-        <v>0.124</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="W3">
         <v>29.292000000000002</v>
@@ -1152,10 +1152,10 @@
         <v>14.898200000000001</v>
       </c>
       <c r="L4">
-        <v>-7.7460000000000004</v>
+        <v>2.3820000000000001</v>
       </c>
       <c r="M4">
-        <v>-5.58</v>
+        <v>2.1920000000000002</v>
       </c>
       <c r="N4">
         <v>133.411</v>
@@ -1179,10 +1179,10 @@
         <v>13.951000000000001</v>
       </c>
       <c r="U4">
-        <v>-0.16700000000000001</v>
+        <v>0.16900000000000001</v>
       </c>
       <c r="V4">
-        <v>0.114</v>
+        <v>6.3E-2</v>
       </c>
       <c r="W4">
         <v>25.59</v>
@@ -1229,10 +1229,10 @@
         <v>14.738000000000001</v>
       </c>
       <c r="L5">
-        <v>-8.2710000000000008</v>
+        <v>1.986</v>
       </c>
       <c r="M5">
-        <v>-8.2520000000000007</v>
+        <v>2.2229999999999999</v>
       </c>
       <c r="N5">
         <v>116.40300000000001</v>
@@ -1256,10 +1256,10 @@
         <v>11.750999999999999</v>
       </c>
       <c r="U5">
-        <v>-5.0000000000000001E-3</v>
+        <v>9.4E-2</v>
       </c>
       <c r="V5">
-        <v>-0.13200000000000001</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="W5">
         <v>20.619</v>
@@ -1306,10 +1306,10 @@
         <v>15.120699999999999</v>
       </c>
       <c r="L6">
-        <v>-0.54700000000000004</v>
+        <v>3.6280000000000001</v>
       </c>
       <c r="M6">
-        <v>8.2240000000000002</v>
+        <v>4.5140000000000002</v>
       </c>
       <c r="N6">
         <v>137.637</v>
@@ -1333,10 +1333,10 @@
         <v>17.45</v>
       </c>
       <c r="U6">
-        <v>-8.1000000000000003E-2</v>
+        <v>-4.0000000000000001E-3</v>
       </c>
       <c r="V6">
-        <v>0.04</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="W6">
         <v>33.194000000000003</v>
@@ -1383,10 +1383,10 @@
         <v>14.758699999999997</v>
       </c>
       <c r="L7">
-        <v>-11.311999999999999</v>
+        <v>0.251</v>
       </c>
       <c r="M7">
-        <v>-10.881</v>
+        <v>0.24299999999999999</v>
       </c>
       <c r="N7">
         <v>97.158000000000001</v>
@@ -1410,10 +1410,10 @@
         <v>10.233000000000001</v>
       </c>
       <c r="U7">
-        <v>-1.4E-2</v>
+        <v>-1.6E-2</v>
       </c>
       <c r="V7">
-        <v>-0.13300000000000001</v>
+        <v>-9.6000000000000002E-2</v>
       </c>
       <c r="W7">
         <v>35.335999999999999</v>
@@ -1460,10 +1460,10 @@
         <v>14.912199999999999</v>
       </c>
       <c r="L8">
-        <v>-12.581</v>
+        <v>0.183</v>
       </c>
       <c r="M8">
-        <v>-12.362</v>
+        <v>0.4</v>
       </c>
       <c r="N8">
         <v>73.341999999999999</v>
@@ -1487,10 +1487,10 @@
         <v>9.1850000000000005</v>
       </c>
       <c r="U8">
-        <v>-3.9E-2</v>
+        <v>0.12</v>
       </c>
       <c r="V8">
-        <v>1.9E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="W8">
         <v>18.556000000000001</v>
@@ -1537,10 +1537,10 @@
         <v>15.236800000000001</v>
       </c>
       <c r="L9">
-        <v>-12.635</v>
+        <v>0.12</v>
       </c>
       <c r="M9">
-        <v>-11.207000000000001</v>
+        <v>0.71899999999999997</v>
       </c>
       <c r="N9">
         <v>41.384999999999998</v>
@@ -1564,10 +1564,10 @@
         <v>11.042999999999999</v>
       </c>
       <c r="U9">
-        <v>-0.20399999999999999</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="V9">
-        <v>-0.06</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="W9">
         <v>12.439</v>
@@ -1614,10 +1614,10 @@
         <v>15.052500000000002</v>
       </c>
       <c r="L10">
-        <v>-12.791</v>
+        <v>0.03</v>
       </c>
       <c r="M10">
-        <v>-11.318</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="N10">
         <v>31.65</v>
@@ -1641,10 +1641,10 @@
         <v>10.161</v>
       </c>
       <c r="U10">
-        <v>-2.8000000000000001E-2</v>
+        <v>-0.02</v>
       </c>
       <c r="V10">
-        <v>2.1999999999999999E-2</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="W10">
         <v>12.071999999999999</v>
@@ -1691,10 +1691,10 @@
         <v>15.2722</v>
       </c>
       <c r="L11">
-        <v>-12.76</v>
+        <v>0.13</v>
       </c>
       <c r="M11">
-        <v>-11.609</v>
+        <v>0.57399999999999995</v>
       </c>
       <c r="N11">
         <v>36.093000000000004</v>
@@ -1718,10 +1718,10 @@
         <v>12.625</v>
       </c>
       <c r="U11">
-        <v>-0.153</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="V11">
-        <v>0.106</v>
+        <v>0.20699999999999999</v>
       </c>
       <c r="W11">
         <v>12.837</v>
@@ -1768,10 +1768,10 @@
         <v>15.037400000000002</v>
       </c>
       <c r="L12">
-        <v>-12.991</v>
+        <v>0.01</v>
       </c>
       <c r="M12">
-        <v>-12.85</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="N12">
         <v>43.052</v>
@@ -1795,10 +1795,10 @@
         <v>13.84</v>
       </c>
       <c r="U12">
-        <v>-1.9E-2</v>
+        <v>0.14099999999999999</v>
       </c>
       <c r="V12">
-        <v>3.4000000000000002E-2</v>
+        <v>7.8E-2</v>
       </c>
       <c r="W12">
         <v>14.324999999999999</v>
@@ -1845,10 +1845,10 @@
         <v>15.088899999999999</v>
       </c>
       <c r="L13">
-        <v>-12.984</v>
+        <v>-1.7999999999999999E-2</v>
       </c>
       <c r="M13">
-        <v>-12.868</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="N13">
         <v>43.401000000000003</v>
@@ -1872,10 +1872,10 @@
         <v>14.948</v>
       </c>
       <c r="U13">
-        <v>0.127</v>
+        <v>0.21</v>
       </c>
       <c r="V13">
-        <v>8.9999999999999993E-3</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="W13">
         <v>14.396000000000001</v>
@@ -1922,10 +1922,10 @@
         <v>14.901999999999999</v>
       </c>
       <c r="L14">
-        <v>-11.853999999999999</v>
+        <v>0.317</v>
       </c>
       <c r="M14">
-        <v>-10.076000000000001</v>
+        <v>1.821</v>
       </c>
       <c r="N14">
         <v>16.265000000000001</v>
@@ -1949,10 +1949,10 @@
         <v>13.052</v>
       </c>
       <c r="U14">
-        <v>-4.7E-2</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="V14">
-        <v>8.6999999999999994E-2</v>
+        <v>0.10299999999999999</v>
       </c>
       <c r="W14">
         <v>9.9589999999999996</v>
@@ -1999,10 +1999,10 @@
         <v>15.2607</v>
       </c>
       <c r="L15">
-        <v>-12.832000000000001</v>
+        <v>0.13900000000000001</v>
       </c>
       <c r="M15">
-        <v>-11.276999999999999</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="N15">
         <v>8.9540000000000006</v>
@@ -2026,10 +2026,10 @@
         <v>23.934000000000001</v>
       </c>
       <c r="U15">
-        <v>0.13100000000000001</v>
+        <v>0.51700000000000002</v>
       </c>
       <c r="V15">
-        <v>0.89700000000000002</v>
+        <v>0.627</v>
       </c>
       <c r="W15">
         <v>11.794</v>
@@ -2076,10 +2076,10 @@
         <v>14.923299999999998</v>
       </c>
       <c r="L16">
-        <v>-12.679</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="M16">
-        <v>-12.432</v>
+        <v>0.26600000000000001</v>
       </c>
       <c r="N16">
         <v>5.1280000000000001</v>
@@ -2103,10 +2103,10 @@
         <v>16.37</v>
       </c>
       <c r="U16">
-        <v>0.10100000000000001</v>
+        <v>0.33800000000000002</v>
       </c>
       <c r="V16">
-        <v>0.48299999999999998</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="W16">
         <v>9.08</v>
@@ -2153,10 +2153,10 @@
         <v>15.205299999999998</v>
       </c>
       <c r="L17">
-        <v>-12.961</v>
+        <v>-0.01</v>
       </c>
       <c r="M17">
-        <v>-12.993</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="N17">
         <v>3.9390000000000001</v>
@@ -2180,10 +2180,10 @@
         <v>24.068000000000001</v>
       </c>
       <c r="U17">
-        <v>0.40699999999999997</v>
+        <v>0.72399999999999998</v>
       </c>
       <c r="V17">
-        <v>0.83499999999999996</v>
+        <v>1.054</v>
       </c>
       <c r="W17">
         <v>9.6430000000000007</v>
@@ -2230,10 +2230,10 @@
         <v>15.1258</v>
       </c>
       <c r="L18">
-        <v>-13.032</v>
+        <v>-6.4000000000000001E-2</v>
       </c>
       <c r="M18">
-        <v>-13.007</v>
+        <v>-5.0999999999999997E-2</v>
       </c>
       <c r="N18">
         <v>0.81699999999999995</v>
@@ -2257,10 +2257,10 @@
         <v>24.908999999999999</v>
       </c>
       <c r="U18">
-        <v>0.56000000000000005</v>
+        <v>0.67100000000000004</v>
       </c>
       <c r="V18">
-        <v>1.0840000000000001</v>
+        <v>1.3009999999999999</v>
       </c>
       <c r="W18">
         <v>8.2330000000000005</v>
@@ -2307,10 +2307,10 @@
         <v>15.284400000000002</v>
       </c>
       <c r="L19">
-        <v>-13.041</v>
+        <v>-4.9000000000000002E-2</v>
       </c>
       <c r="M19">
-        <v>-13.063000000000001</v>
+        <v>-6.2E-2</v>
       </c>
       <c r="N19">
         <v>0.221</v>
@@ -2334,10 +2334,10 @@
         <v>12.452</v>
       </c>
       <c r="U19">
-        <v>0.217</v>
+        <v>0.374</v>
       </c>
       <c r="V19">
-        <v>9.7000000000000003E-2</v>
+        <v>0.57499999999999996</v>
       </c>
       <c r="W19">
         <v>2.6920000000000002</v>
@@ -2384,10 +2384,10 @@
         <v>15.025099999999998</v>
       </c>
       <c r="L20">
-        <v>-12.85</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M20">
-        <v>-12.818</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="N20">
         <v>24.209</v>
@@ -2411,10 +2411,10 @@
         <v>18.132000000000001</v>
       </c>
       <c r="U20">
-        <v>0.33900000000000002</v>
+        <v>1.4079999999999999</v>
       </c>
       <c r="V20">
-        <v>0.60399999999999998</v>
+        <v>2.0049999999999999</v>
       </c>
       <c r="W20">
         <v>16.34</v>
@@ -2461,10 +2461,10 @@
         <v>15.094200000000001</v>
       </c>
       <c r="L21">
-        <v>-12.94</v>
+        <v>-1.4E-2</v>
       </c>
       <c r="M21">
-        <v>-12.706</v>
+        <v>0.06</v>
       </c>
       <c r="N21">
         <v>22.242000000000001</v>
@@ -2488,10 +2488,10 @@
         <v>20.276</v>
       </c>
       <c r="U21">
-        <v>0.40799999999999997</v>
+        <v>1.1180000000000001</v>
       </c>
       <c r="V21">
-        <v>0.13100000000000001</v>
+        <v>1.4059999999999999</v>
       </c>
       <c r="W21">
         <v>15.42</v>
@@ -2538,10 +2538,10 @@
         <v>15.243599999999999</v>
       </c>
       <c r="L22">
-        <v>-12.988</v>
+        <v>-1.9E-2</v>
       </c>
       <c r="M22">
-        <v>-12.765000000000001</v>
+        <v>3.9E-2</v>
       </c>
       <c r="N22">
         <v>20.831</v>
@@ -2565,10 +2565,10 @@
         <v>24.193999999999999</v>
       </c>
       <c r="U22">
-        <v>-4.1000000000000002E-2</v>
+        <v>0.62</v>
       </c>
       <c r="V22">
-        <v>0.47</v>
+        <v>1.1120000000000001</v>
       </c>
       <c r="W22">
         <v>17.61</v>
@@ -2615,10 +2615,10 @@
         <v>15.250799999999998</v>
       </c>
       <c r="L23">
-        <v>-12.956</v>
+        <v>-8.9999999999999993E-3</v>
       </c>
       <c r="M23">
-        <v>-12.805999999999999</v>
+        <v>1.9E-2</v>
       </c>
       <c r="N23">
         <v>19.768000000000001</v>
@@ -2642,10 +2642,10 @@
         <v>22.85</v>
       </c>
       <c r="U23">
-        <v>0.34200000000000003</v>
+        <v>1.3089999999999999</v>
       </c>
       <c r="V23">
-        <v>0.6</v>
+        <v>1.1890000000000001</v>
       </c>
       <c r="W23">
         <v>13.815</v>
@@ -2692,10 +2692,10 @@
         <v>15.025999999999998</v>
       </c>
       <c r="L24">
-        <v>-12.968999999999999</v>
+        <v>2.7E-2</v>
       </c>
       <c r="M24">
-        <v>-12.778</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="N24">
         <v>14.26</v>
@@ -2719,10 +2719,10 @@
         <v>19.588999999999999</v>
       </c>
       <c r="U24">
-        <v>0.60099999999999998</v>
+        <v>1.173</v>
       </c>
       <c r="V24">
-        <v>0.49</v>
+        <v>1.2430000000000001</v>
       </c>
       <c r="W24">
         <v>9.6069999999999993</v>
@@ -2769,10 +2769,10 @@
         <v>15.2098</v>
       </c>
       <c r="L25">
-        <v>-12.978</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="M25">
-        <v>-12.909000000000001</v>
+        <v>-2E-3</v>
       </c>
       <c r="N25">
         <v>12.211</v>
@@ -2796,10 +2796,10 @@
         <v>24.190999999999999</v>
       </c>
       <c r="U25">
-        <v>0.253</v>
+        <v>1.1319999999999999</v>
       </c>
       <c r="V25">
-        <v>0.157</v>
+        <v>1.1479999999999999</v>
       </c>
       <c r="W25">
         <v>10.092000000000001</v>
@@ -2846,10 +2846,10 @@
         <v>15.081199999999999</v>
       </c>
       <c r="L26">
-        <v>-13.026</v>
+        <v>-0.02</v>
       </c>
       <c r="M26">
-        <v>-13.010999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="N26">
         <v>6.2380000000000004</v>
@@ -2873,10 +2873,10 @@
         <v>24.140999999999998</v>
       </c>
       <c r="U26">
-        <v>0.08</v>
+        <v>0.66700000000000004</v>
       </c>
       <c r="V26">
-        <v>9.5000000000000001E-2</v>
+        <v>0.72099999999999997</v>
       </c>
       <c r="W26">
         <v>9.3260000000000005</v>
@@ -2923,10 +2923,10 @@
         <v>14.904999999999999</v>
       </c>
       <c r="L27">
-        <v>-13.031000000000001</v>
+        <v>-3.5999999999999997E-2</v>
       </c>
       <c r="M27">
-        <v>-13.022</v>
+        <v>-4.2999999999999997E-2</v>
       </c>
       <c r="N27">
         <v>4.9649999999999999</v>
@@ -2950,10 +2950,10 @@
         <v>20.318999999999999</v>
       </c>
       <c r="U27">
-        <v>0.20399999999999999</v>
+        <v>0.90400000000000003</v>
       </c>
       <c r="V27">
-        <v>0.19800000000000001</v>
+        <v>0.78300000000000003</v>
       </c>
       <c r="W27">
         <v>7.508</v>
@@ -3000,10 +3000,10 @@
         <v>15.1996</v>
       </c>
       <c r="L28">
-        <v>-13.032</v>
+        <v>-5.3999999999999999E-2</v>
       </c>
       <c r="M28">
-        <v>-13.048</v>
+        <v>-4.4999999999999998E-2</v>
       </c>
       <c r="N28">
         <v>3.1890000000000001</v>
@@ -3027,10 +3027,10 @@
         <v>28.100999999999999</v>
       </c>
       <c r="U28">
-        <v>0.17399999999999999</v>
+        <v>1.0669999999999999</v>
       </c>
       <c r="V28">
-        <v>0.23300000000000001</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="W28">
         <v>9.4670000000000005</v>
@@ -3077,10 +3077,10 @@
         <v>14.971399999999999</v>
       </c>
       <c r="L29">
-        <v>-13.029</v>
+        <v>-2.5999999999999999E-2</v>
       </c>
       <c r="M29">
-        <v>-13.019</v>
+        <v>-3.9E-2</v>
       </c>
       <c r="N29">
         <v>2.63</v>
@@ -3104,10 +3104,10 @@
         <v>21.888000000000002</v>
       </c>
       <c r="U29">
-        <v>0.45800000000000002</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="V29">
-        <v>8.6999999999999994E-2</v>
+        <v>0.93100000000000005</v>
       </c>
       <c r="W29">
         <v>6.7779999999999996</v>
@@ -3154,10 +3154,10 @@
         <v>14.785600000000001</v>
       </c>
       <c r="L30">
-        <v>-13.045</v>
+        <v>-2.4E-2</v>
       </c>
       <c r="M30">
-        <v>-13.016999999999999</v>
+        <v>-3.7999999999999999E-2</v>
       </c>
       <c r="N30">
         <v>1.927</v>
@@ -3181,10 +3181,10 @@
         <v>13.957000000000001</v>
       </c>
       <c r="U30">
-        <v>0.67200000000000004</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="V30">
-        <v>0.72299999999999998</v>
+        <v>0.89800000000000002</v>
       </c>
       <c r="W30">
         <v>5.3</v>
@@ -3231,10 +3231,10 @@
         <v>14.8368</v>
       </c>
       <c r="L31">
-        <v>-13.065</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="M31">
-        <v>-13.028</v>
+        <v>-3.9E-2</v>
       </c>
       <c r="N31">
         <v>1.982</v>
@@ -3258,10 +3258,10 @@
         <v>15.218</v>
       </c>
       <c r="U31">
-        <v>5.5E-2</v>
+        <v>0.27900000000000003</v>
       </c>
       <c r="V31">
-        <v>0.17399999999999999</v>
+        <v>0.68600000000000005</v>
       </c>
       <c r="W31">
         <v>5.52</v>
@@ -3308,10 +3308,10 @@
         <v>14.933</v>
       </c>
       <c r="L32">
-        <v>-13.042999999999999</v>
+        <v>-4.4999999999999998E-2</v>
       </c>
       <c r="M32">
-        <v>-13.035</v>
+        <v>-7.2999999999999995E-2</v>
       </c>
       <c r="N32">
         <v>3.2309999999999999</v>
@@ -3335,10 +3335,10 @@
         <v>22.251999999999999</v>
       </c>
       <c r="U32">
-        <v>0.65200000000000002</v>
+        <v>0.51700000000000002</v>
       </c>
       <c r="V32">
-        <v>0.38200000000000001</v>
+        <v>1.0009999999999999</v>
       </c>
       <c r="W32">
         <v>7.7240000000000002</v>
@@ -3385,10 +3385,10 @@
         <v>14.682400000000001</v>
       </c>
       <c r="L33">
-        <v>-13.061</v>
+        <v>-5.5E-2</v>
       </c>
       <c r="M33">
-        <v>-13.037000000000001</v>
+        <v>-5.8000000000000003E-2</v>
       </c>
       <c r="N33">
         <v>1.3779999999999999</v>
@@ -3412,10 +3412,10 @@
         <v>14.414999999999999</v>
       </c>
       <c r="U33">
-        <v>0.153</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="V33">
-        <v>0.38300000000000001</v>
+        <v>0.65500000000000003</v>
       </c>
       <c r="W33">
         <v>4.891</v>
@@ -3462,10 +3462,10 @@
         <v>14.590199999999999</v>
       </c>
       <c r="L34">
-        <v>-13.057</v>
+        <v>-4.4999999999999998E-2</v>
       </c>
       <c r="M34">
-        <v>-13.023999999999999</v>
+        <v>-3.4000000000000002E-2</v>
       </c>
       <c r="N34">
         <v>1.367</v>
@@ -3489,10 +3489,10 @@
         <v>10.893000000000001</v>
       </c>
       <c r="U34">
-        <v>0.20599999999999999</v>
+        <v>0.29399999999999998</v>
       </c>
       <c r="V34">
-        <v>0.45</v>
+        <v>0.94799999999999995</v>
       </c>
       <c r="W34">
         <v>3.7869999999999999</v>
@@ -3539,10 +3539,10 @@
         <v>15.011900000000001</v>
       </c>
       <c r="L35">
-        <v>-13.055999999999999</v>
+        <v>-0.03</v>
       </c>
       <c r="M35">
-        <v>-13.019</v>
+        <v>-3.2000000000000001E-2</v>
       </c>
       <c r="N35">
         <v>1.4490000000000001</v>
@@ -3566,10 +3566,10 @@
         <v>22.13</v>
       </c>
       <c r="U35">
-        <v>0.59399999999999997</v>
+        <v>0.628</v>
       </c>
       <c r="V35">
-        <v>0.58199999999999996</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="W35">
         <v>8.5350000000000001</v>
@@ -3616,10 +3616,10 @@
         <v>14.680699999999998</v>
       </c>
       <c r="L36">
-        <v>-13.041</v>
+        <v>-5.1999999999999998E-2</v>
       </c>
       <c r="M36">
-        <v>-13.05</v>
+        <v>-5.1999999999999998E-2</v>
       </c>
       <c r="N36">
         <v>0.41</v>
@@ -3643,10 +3643,10 @@
         <v>12.292999999999999</v>
       </c>
       <c r="U36">
-        <v>0.41899999999999998</v>
+        <v>0.40300000000000002</v>
       </c>
       <c r="V36">
-        <v>0.52700000000000002</v>
+        <v>0.61799999999999999</v>
       </c>
       <c r="W36">
         <v>4.0869999999999997</v>
@@ -3693,10 +3693,10 @@
         <v>14.7074</v>
       </c>
       <c r="L37">
-        <v>-10.478</v>
+        <v>1.6659999999999999</v>
       </c>
       <c r="M37">
-        <v>-6.2430000000000003</v>
+        <v>2.7040000000000002</v>
       </c>
       <c r="N37">
         <v>100.44</v>
@@ -3720,10 +3720,10 @@
         <v>9.0020000000000007</v>
       </c>
       <c r="U37">
-        <v>-8.4000000000000005E-2</v>
+        <v>0.188</v>
       </c>
       <c r="V37">
-        <v>3.1E-2</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="W37">
         <v>11.433</v>
@@ -3770,10 +3770,10 @@
         <v>14.7759</v>
       </c>
       <c r="L38">
-        <v>-7.84</v>
+        <v>3.7829999999999999</v>
       </c>
       <c r="M38">
-        <v>-1.5449999999999999</v>
+        <v>6.8040000000000003</v>
       </c>
       <c r="N38">
         <v>98.900999999999996</v>
@@ -3797,10 +3797,10 @@
         <v>13.195</v>
       </c>
       <c r="U38">
-        <v>-0.112</v>
+        <v>1.9E-2</v>
       </c>
       <c r="V38">
-        <v>-0.16200000000000001</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="W38">
         <v>15.206</v>
@@ -3847,10 +3847,10 @@
         <v>14.754999999999999</v>
       </c>
       <c r="L39">
-        <v>-6.8710000000000004</v>
+        <v>3.214</v>
       </c>
       <c r="M39">
-        <v>-4.9630000000000001</v>
+        <v>3.2570000000000001</v>
       </c>
       <c r="N39">
         <v>119.38500000000001</v>
@@ -3874,10 +3874,10 @@
         <v>11.454000000000001</v>
       </c>
       <c r="U39">
-        <v>-4.0000000000000001E-3</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="V39">
-        <v>-0.111</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="W39">
         <v>17.41</v>
@@ -3924,10 +3924,10 @@
         <v>14.553899999999999</v>
       </c>
       <c r="L40">
-        <v>-8.7200000000000006</v>
+        <v>2.387</v>
       </c>
       <c r="M40">
-        <v>-11.621</v>
+        <v>0.35499999999999998</v>
       </c>
       <c r="N40">
         <v>105.664</v>
@@ -3951,10 +3951,10 @@
         <v>7.1260000000000003</v>
       </c>
       <c r="U40">
-        <v>4.0000000000000001E-3</v>
+        <v>-0.10299999999999999</v>
       </c>
       <c r="V40">
-        <v>-0.252</v>
+        <v>3.9E-2</v>
       </c>
       <c r="W40">
         <v>14.255000000000001</v>
@@ -4001,10 +4001,10 @@
         <v>14.4176</v>
       </c>
       <c r="L41">
-        <v>-9.4450000000000003</v>
+        <v>2.3879999999999999</v>
       </c>
       <c r="M41">
-        <v>8.3000000000000004E-2</v>
+        <v>8.5830000000000002</v>
       </c>
       <c r="N41">
         <v>105.855</v>
@@ -4028,10 +4028,10 @@
         <v>6.1790000000000003</v>
       </c>
       <c r="U41">
-        <v>-0.14099999999999999</v>
+        <v>-0.02</v>
       </c>
       <c r="V41">
-        <v>-0.107</v>
+        <v>-0.01</v>
       </c>
       <c r="W41">
         <v>13.076000000000001</v>
@@ -4078,10 +4078,10 @@
         <v>14.897299999999998</v>
       </c>
       <c r="L42">
-        <v>-2.242</v>
+        <v>7.8330000000000002</v>
       </c>
       <c r="M42">
-        <v>4.6989999999999998</v>
+        <v>11.791</v>
       </c>
       <c r="N42">
         <v>163.398</v>
@@ -4105,10 +4105,10 @@
         <v>17.04</v>
       </c>
       <c r="U42">
-        <v>4.0000000000000001E-3</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="V42">
-        <v>3.1E-2</v>
+        <v>9.0999999999999998E-2</v>
       </c>
       <c r="W42">
         <v>21.199000000000002</v>
@@ -4155,10 +4155,10 @@
         <v>14.8582</v>
       </c>
       <c r="L43">
-        <v>-3.9409999999999998</v>
+        <v>3.2869999999999999</v>
       </c>
       <c r="M43">
-        <v>10.635</v>
+        <v>17.385999999999999</v>
       </c>
       <c r="N43">
         <v>135.185</v>
@@ -4182,10 +4182,10 @@
         <v>17.873000000000001</v>
       </c>
       <c r="U43">
-        <v>-0.108</v>
+        <v>7.2999999999999995E-2</v>
       </c>
       <c r="V43">
-        <v>-9.2999999999999999E-2</v>
+        <v>-9.9000000000000005E-2</v>
       </c>
       <c r="W43">
         <v>21.181000000000001</v>
@@ -4232,10 +4232,10 @@
         <v>14.691099999999999</v>
       </c>
       <c r="L44">
-        <v>-9.5830000000000002</v>
+        <v>0.72699999999999998</v>
       </c>
       <c r="M44">
-        <v>-6.8319999999999999</v>
+        <v>1.7270000000000001</v>
       </c>
       <c r="N44">
         <v>101.836</v>
@@ -4259,10 +4259,10 @@
         <v>11.696999999999999</v>
       </c>
       <c r="U44">
-        <v>-3.1E-2</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="V44">
-        <v>-0.14499999999999999</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="W44">
         <v>24.949000000000002</v>
@@ -4309,10 +4309,10 @@
         <v>14.587699999999998</v>
       </c>
       <c r="L45">
-        <v>-11.968999999999999</v>
+        <v>0.13800000000000001</v>
       </c>
       <c r="M45">
-        <v>-4.5289999999999999</v>
+        <v>3.0150000000000001</v>
       </c>
       <c r="N45">
         <v>92.775999999999996</v>
@@ -4336,10 +4336,10 @@
         <v>6.968</v>
       </c>
       <c r="U45">
-        <v>0.20599999999999999</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="V45">
-        <v>2.5000000000000001E-2</v>
+        <v>-5.6000000000000001E-2</v>
       </c>
       <c r="W45">
         <v>16.763999999999999</v>
@@ -4386,10 +4386,10 @@
         <v>14.871199999999998</v>
       </c>
       <c r="L46">
-        <v>-10.99</v>
+        <v>1.385</v>
       </c>
       <c r="M46">
-        <v>-2.6509999999999998</v>
+        <v>4.968</v>
       </c>
       <c r="N46">
         <v>83.100999999999999</v>
@@ -4413,10 +4413,10 @@
         <v>12.666</v>
       </c>
       <c r="U46">
-        <v>-5.0000000000000001E-3</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="V46">
-        <v>-1.0999999999999999E-2</v>
+        <v>0.13400000000000001</v>
       </c>
       <c r="W46">
         <v>16.183</v>
@@ -4463,10 +4463,10 @@
         <v>15.425099999999999</v>
       </c>
       <c r="L47">
-        <v>-12.773999999999999</v>
+        <v>0.126</v>
       </c>
       <c r="M47">
-        <v>-8.5559999999999992</v>
+        <v>2.5750000000000002</v>
       </c>
       <c r="N47">
         <v>31.529</v>
@@ -4490,10 +4490,10 @@
         <v>23.792000000000002</v>
       </c>
       <c r="U47">
-        <v>0.17100000000000001</v>
+        <v>0.1</v>
       </c>
       <c r="V47">
-        <v>5.3999999999999999E-2</v>
+        <v>0.14199999999999999</v>
       </c>
       <c r="W47">
         <v>13.228999999999999</v>
@@ -4540,10 +4540,10 @@
         <v>15.188699999999999</v>
       </c>
       <c r="L48">
-        <v>-12.701000000000001</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="M48">
-        <v>-10.151999999999999</v>
+        <v>1.319</v>
       </c>
       <c r="N48">
         <v>25.132000000000001</v>
@@ -4567,10 +4567,10 @@
         <v>20.681999999999999</v>
       </c>
       <c r="U48">
-        <v>7.2999999999999995E-2</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="V48">
-        <v>8.5000000000000006E-2</v>
+        <v>5.2999999999999999E-2</v>
       </c>
       <c r="W48">
         <v>11.407999999999999</v>
@@ -4617,10 +4617,10 @@
         <v>15.155299999999999</v>
       </c>
       <c r="L49">
-        <v>-12.773</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="M49">
-        <v>-9.6010000000000009</v>
+        <v>1.399</v>
       </c>
       <c r="N49">
         <v>12.829000000000001</v>
@@ -4644,10 +4644,10 @@
         <v>19.539000000000001</v>
       </c>
       <c r="U49">
-        <v>-4.8000000000000001E-2</v>
+        <v>0.34399999999999997</v>
       </c>
       <c r="V49">
-        <v>0.27200000000000002</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="W49">
         <v>9.4019999999999992</v>
@@ -4694,10 +4694,10 @@
         <v>15.273499999999999</v>
       </c>
       <c r="L50">
-        <v>-12.927</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M50">
-        <v>-11.896000000000001</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="N50">
         <v>14.132999999999999</v>
@@ -4721,10 +4721,10 @@
         <v>24.041</v>
       </c>
       <c r="U50">
-        <v>-8.7999999999999995E-2</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="V50">
-        <v>0.11899999999999999</v>
+        <v>0.24</v>
       </c>
       <c r="W50">
         <v>9.5760000000000005</v>
@@ -4771,10 +4771,10 @@
         <v>15.4001</v>
       </c>
       <c r="L51">
-        <v>-12.973000000000001</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="M51">
-        <v>-12.436</v>
+        <v>0.3</v>
       </c>
       <c r="N51">
         <v>5.8780000000000001</v>
@@ -4798,10 +4798,10 @@
         <v>31.401</v>
       </c>
       <c r="U51">
-        <v>-0.10199999999999999</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="V51">
-        <v>0.249</v>
+        <v>0.88300000000000001</v>
       </c>
       <c r="W51">
         <v>10.875</v>
@@ -4848,10 +4848,10 @@
         <v>15.122300000000003</v>
       </c>
       <c r="L52">
-        <v>-13.021000000000001</v>
+        <v>2E-3</v>
       </c>
       <c r="M52">
-        <v>-12.663</v>
+        <v>0.18</v>
       </c>
       <c r="N52">
         <v>2.4820000000000002</v>
@@ -4875,10 +4875,10 @@
         <v>25.567</v>
       </c>
       <c r="U52">
-        <v>0.28799999999999998</v>
+        <v>1.056</v>
       </c>
       <c r="V52">
-        <v>0.17699999999999999</v>
+        <v>0.52200000000000002</v>
       </c>
       <c r="W52">
         <v>8.6240000000000006</v>
@@ -4925,10 +4925,10 @@
         <v>15.154500000000001</v>
       </c>
       <c r="L53">
-        <v>-13.005000000000001</v>
+        <v>-0.01</v>
       </c>
       <c r="M53">
-        <v>-13.021000000000001</v>
+        <v>0</v>
       </c>
       <c r="N53">
         <v>2.081</v>
@@ -4952,10 +4952,10 @@
         <v>30.613</v>
       </c>
       <c r="U53">
-        <v>0.66700000000000004</v>
+        <v>1.3580000000000001</v>
       </c>
       <c r="V53">
-        <v>0.66100000000000003</v>
+        <v>1.4179999999999999</v>
       </c>
       <c r="W53">
         <v>10.483000000000001</v>
@@ -5002,10 +5002,10 @@
         <v>14.733000000000001</v>
       </c>
       <c r="L54">
-        <v>-13.023</v>
+        <v>-2.1999999999999999E-2</v>
       </c>
       <c r="M54">
-        <v>-13.058999999999999</v>
+        <v>-0.04</v>
       </c>
       <c r="N54">
         <v>0.874</v>
@@ -5029,10 +5029,10 @@
         <v>15.379</v>
       </c>
       <c r="U54">
-        <v>0.94399999999999995</v>
+        <v>1.054</v>
       </c>
       <c r="V54">
-        <v>0.79100000000000004</v>
+        <v>1.079</v>
       </c>
       <c r="W54">
         <v>4.8769999999999998</v>
@@ -5079,10 +5079,10 @@
         <v>14.903700000000001</v>
       </c>
       <c r="L55">
-        <v>-12.827999999999999</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="M55">
-        <v>-25.597000000000001</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="N55">
         <v>15.35</v>
@@ -5106,10 +5106,10 @@
         <v>12.33</v>
       </c>
       <c r="U55">
-        <v>1.3540000000000001</v>
+        <v>1.65</v>
       </c>
       <c r="V55">
-        <v>1.363</v>
+        <v>1.619</v>
       </c>
       <c r="W55">
         <v>15.199</v>
@@ -5156,10 +5156,10 @@
         <v>14.677299999999999</v>
       </c>
       <c r="L56">
-        <v>-12.706</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="M56">
-        <v>-24.3</v>
+        <v>0.372</v>
       </c>
       <c r="N56">
         <v>10.26</v>
@@ -5183,10 +5183,10 @@
         <v>8.7550000000000008</v>
       </c>
       <c r="U56">
-        <v>0.64500000000000002</v>
+        <v>0.90400000000000003</v>
       </c>
       <c r="V56">
-        <v>0.91600000000000004</v>
+        <v>1.1040000000000001</v>
       </c>
       <c r="W56">
         <v>8.5310000000000006</v>
@@ -5233,10 +5233,10 @@
         <v>14.8786</v>
       </c>
       <c r="L57">
-        <v>-12.728</v>
+        <v>0.17699999999999999</v>
       </c>
       <c r="M57">
-        <v>-24.391999999999999</v>
+        <v>0.38700000000000001</v>
       </c>
       <c r="N57">
         <v>9.3219999999999992</v>
@@ -5260,10 +5260,10 @@
         <v>11.53</v>
       </c>
       <c r="U57">
-        <v>0.52100000000000002</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="V57">
-        <v>0.94199999999999995</v>
+        <v>0.996</v>
       </c>
       <c r="W57">
         <v>10.294</v>
@@ -5310,10 +5310,10 @@
         <v>14.7849</v>
       </c>
       <c r="L58">
-        <v>-12.840999999999999</v>
+        <v>0.16200000000000001</v>
       </c>
       <c r="M58">
-        <v>-25.568000000000001</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="N58">
         <v>11.004</v>
@@ -5337,10 +5337,10 @@
         <v>10.708</v>
       </c>
       <c r="U58">
-        <v>0.38500000000000001</v>
+        <v>0.85599999999999998</v>
       </c>
       <c r="V58">
-        <v>0.60899999999999999</v>
+        <v>1.044</v>
       </c>
       <c r="W58">
         <v>8.3260000000000005</v>
@@ -5387,10 +5387,10 @@
         <v>14.799800000000001</v>
       </c>
       <c r="L59">
-        <v>-12.712999999999999</v>
+        <v>0.17499999999999999</v>
       </c>
       <c r="M59">
-        <v>-24.774999999999999</v>
+        <v>0.29899999999999999</v>
       </c>
       <c r="N59">
         <v>9.2829999999999995</v>
@@ -5414,10 +5414,10 @@
         <v>12.319000000000001</v>
       </c>
       <c r="U59">
-        <v>0.55200000000000005</v>
+        <v>0.92500000000000004</v>
       </c>
       <c r="V59">
-        <v>0.78700000000000003</v>
+        <v>1.2549999999999999</v>
       </c>
       <c r="W59">
         <v>9.1259999999999994</v>
@@ -5464,10 +5464,10 @@
         <v>14.823399999999999</v>
       </c>
       <c r="L60">
-        <v>-12.821999999999999</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="M60">
-        <v>-24.776</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="N60">
         <v>7.7869999999999999</v>
@@ -5491,10 +5491,10 @@
         <v>13.695</v>
       </c>
       <c r="U60">
-        <v>0.63600000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="V60">
-        <v>0.68100000000000005</v>
+        <v>0.80400000000000005</v>
       </c>
       <c r="W60">
         <v>9.36</v>
@@ -5541,10 +5541,10 @@
         <v>14.7715</v>
       </c>
       <c r="L61">
-        <v>-12.869</v>
+        <v>8.1000000000000003E-2</v>
       </c>
       <c r="M61">
-        <v>-25.306999999999999</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="N61">
         <v>8.7349999999999994</v>
@@ -5568,10 +5568,10 @@
         <v>11.177</v>
       </c>
       <c r="U61">
-        <v>0.44400000000000001</v>
+        <v>0.49399999999999999</v>
       </c>
       <c r="V61">
-        <v>0.76700000000000002</v>
+        <v>1.0660000000000001</v>
       </c>
       <c r="W61">
         <v>7.181</v>
@@ -5618,10 +5618,10 @@
         <v>15.049900000000001</v>
       </c>
       <c r="L62">
-        <v>-12.866</v>
+        <v>8.7999999999999995E-2</v>
       </c>
       <c r="M62">
-        <v>-25.283999999999999</v>
+        <v>0.187</v>
       </c>
       <c r="N62">
         <v>6.5510000000000002</v>
@@ -5645,10 +5645,10 @@
         <v>16.518999999999998</v>
       </c>
       <c r="U62">
-        <v>0.78200000000000003</v>
+        <v>0.95799999999999996</v>
       </c>
       <c r="V62">
-        <v>0.626</v>
+        <v>0.73599999999999999</v>
       </c>
       <c r="W62">
         <v>10.648999999999999</v>
@@ -5695,10 +5695,10 @@
         <v>15.034500000000001</v>
       </c>
       <c r="L63">
-        <v>-12.829000000000001</v>
+        <v>0.12</v>
       </c>
       <c r="M63">
-        <v>-25.023</v>
+        <v>0.2</v>
       </c>
       <c r="N63">
         <v>7.7619999999999996</v>
@@ -5722,10 +5722,10 @@
         <v>21.111999999999998</v>
       </c>
       <c r="U63">
-        <v>0.91500000000000004</v>
+        <v>1.2410000000000001</v>
       </c>
       <c r="V63">
-        <v>0.89300000000000002</v>
+        <v>1.0980000000000001</v>
       </c>
       <c r="W63">
         <v>13.705</v>
@@ -5772,10 +5772,10 @@
         <v>14.8817</v>
       </c>
       <c r="L64">
-        <v>-12.802</v>
+        <v>0.121</v>
       </c>
       <c r="M64">
-        <v>-25.256</v>
+        <v>0.221</v>
       </c>
       <c r="N64">
         <v>5.3520000000000003</v>
@@ -5799,10 +5799,10 @@
         <v>19.245000000000001</v>
       </c>
       <c r="U64">
-        <v>0.54100000000000004</v>
+        <v>0.92100000000000004</v>
       </c>
       <c r="V64">
-        <v>0.82399999999999995</v>
+        <v>1.181</v>
       </c>
       <c r="W64">
         <v>10.766999999999999</v>
@@ -5849,10 +5849,10 @@
         <v>15.2197</v>
       </c>
       <c r="L65">
-        <v>-12.907</v>
+        <v>7.8E-2</v>
       </c>
       <c r="M65">
-        <v>-25.094999999999999</v>
+        <v>0.252</v>
       </c>
       <c r="N65">
         <v>7.6120000000000001</v>
@@ -5876,10 +5876,10 @@
         <v>24.736999999999998</v>
       </c>
       <c r="U65">
-        <v>0.40899999999999997</v>
+        <v>0.995</v>
       </c>
       <c r="V65">
-        <v>0.72499999999999998</v>
+        <v>1.2629999999999999</v>
       </c>
       <c r="W65">
         <v>14.218</v>
@@ -5926,10 +5926,10 @@
         <v>15.032</v>
       </c>
       <c r="L66">
-        <v>-12.845000000000001</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="M66">
-        <v>-25.347000000000001</v>
+        <v>0.21199999999999999</v>
       </c>
       <c r="N66">
         <v>6.6840000000000002</v>
@@ -5953,10 +5953,10 @@
         <v>22.224</v>
       </c>
       <c r="U66">
-        <v>0.41199999999999998</v>
+        <v>1.2490000000000001</v>
       </c>
       <c r="V66">
-        <v>0.32</v>
+        <v>1.0620000000000001</v>
       </c>
       <c r="W66">
         <v>12.510999999999999</v>
@@ -6003,10 +6003,10 @@
         <v>15.064</v>
       </c>
       <c r="L67">
-        <v>-12.884</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="M67">
-        <v>-25.733000000000001</v>
+        <v>0.157</v>
       </c>
       <c r="N67">
         <v>2.589</v>
@@ -6030,10 +6030,10 @@
         <v>21.303000000000001</v>
       </c>
       <c r="U67">
-        <v>0.73299999999999998</v>
+        <v>0.93700000000000006</v>
       </c>
       <c r="V67">
-        <v>0.58499999999999996</v>
+        <v>0.73499999999999999</v>
       </c>
       <c r="W67">
         <v>9.4610000000000003</v>
@@ -6080,10 +6080,10 @@
         <v>14.6785</v>
       </c>
       <c r="L68">
-        <v>-12.896000000000001</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="M68">
-        <v>-25.664999999999999</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="N68">
         <v>3.5880000000000001</v>
@@ -6107,10 +6107,10 @@
         <v>14.721</v>
       </c>
       <c r="U68">
-        <v>0.29599999999999999</v>
+        <v>0.35799999999999998</v>
       </c>
       <c r="V68">
-        <v>-0.23300000000000001</v>
+        <v>0.58399999999999996</v>
       </c>
       <c r="W68">
         <v>6.2709999999999999</v>
@@ -6157,10 +6157,10 @@
         <v>14.717600000000001</v>
       </c>
       <c r="L69">
-        <v>-12.901999999999999</v>
+        <v>4.7E-2</v>
       </c>
       <c r="M69">
-        <v>-25.695</v>
+        <v>0.191</v>
       </c>
       <c r="N69">
         <v>2.8119999999999998</v>
@@ -6184,10 +6184,10 @@
         <v>11.785</v>
       </c>
       <c r="U69">
-        <v>0.45800000000000002</v>
+        <v>0.76300000000000001</v>
       </c>
       <c r="V69">
-        <v>0.437</v>
+        <v>0.52</v>
       </c>
       <c r="W69">
         <v>4.9210000000000003</v>
@@ -6234,10 +6234,10 @@
         <v>14.6022</v>
       </c>
       <c r="L70">
-        <v>-12.972</v>
+        <v>-1.7999999999999999E-2</v>
       </c>
       <c r="M70">
-        <v>-25.937000000000001</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="N70">
         <v>2.452</v>
@@ -6261,10 +6261,10 @@
         <v>10.366</v>
       </c>
       <c r="U70">
-        <v>0.65300000000000002</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="V70">
-        <v>0.151</v>
+        <v>0.67800000000000005</v>
       </c>
       <c r="W70">
         <v>5.0970000000000004</v>
@@ -6311,10 +6311,10 @@
         <v>14.698700000000001</v>
       </c>
       <c r="L71">
-        <v>-12.986000000000001</v>
+        <v>-1.7000000000000001E-2</v>
       </c>
       <c r="M71">
-        <v>-25.850999999999999</v>
+        <v>0.01</v>
       </c>
       <c r="N71">
         <v>2.7570000000000001</v>
@@ -6338,10 +6338,10 @@
         <v>14.265000000000001</v>
       </c>
       <c r="U71">
-        <v>0.186</v>
+        <v>0.66</v>
       </c>
       <c r="V71">
-        <v>0.22</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="W71">
         <v>11.544</v>
@@ -6388,10 +6388,10 @@
         <v>14.855899999999998</v>
       </c>
       <c r="L72">
-        <v>-13.007999999999999</v>
+        <v>2E-3</v>
       </c>
       <c r="M72">
-        <v>-25.905000000000001</v>
+        <v>5.8000000000000003E-2</v>
       </c>
       <c r="N72">
         <v>2.2320000000000002</v>
@@ -6415,10 +6415,10 @@
         <v>16.853999999999999</v>
       </c>
       <c r="U72">
-        <v>0.46300000000000002</v>
+        <v>0.68700000000000006</v>
       </c>
       <c r="V72">
-        <v>0.56399999999999995</v>
+        <v>0.98799999999999999</v>
       </c>
       <c r="W72">
         <v>6.8070000000000004</v>
@@ -6465,10 +6465,10 @@
         <v>14.944800000000001</v>
       </c>
       <c r="L73">
-        <v>-12.996</v>
+        <v>-2.8000000000000001E-2</v>
       </c>
       <c r="M73">
-        <v>-26.024000000000001</v>
+        <v>-1.2999999999999999E-2</v>
       </c>
       <c r="N73">
         <v>1.4770000000000001</v>
@@ -6492,10 +6492,10 @@
         <v>15.907</v>
       </c>
       <c r="U73">
-        <v>0.36399999999999999</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="V73">
-        <v>0.79200000000000004</v>
+        <v>0.92600000000000005</v>
       </c>
       <c r="W73">
         <v>5.68</v>
@@ -6542,10 +6542,10 @@
         <v>14.900599999999999</v>
       </c>
       <c r="L74">
-        <v>-13.053000000000001</v>
+        <v>-2.1000000000000001E-2</v>
       </c>
       <c r="M74">
-        <v>-26.021999999999998</v>
+        <v>-5.5E-2</v>
       </c>
       <c r="N74">
         <v>0.39300000000000002</v>
@@ -6569,10 +6569,10 @@
         <v>14.962</v>
       </c>
       <c r="U74">
-        <v>0.74299999999999999</v>
+        <v>0.58799999999999997</v>
       </c>
       <c r="V74">
-        <v>0.99399999999999999</v>
+        <v>0.71199999999999997</v>
       </c>
       <c r="W74">
         <v>4.1589999999999998</v>
@@ -6619,10 +6619,10 @@
         <v>14.834199999999999</v>
       </c>
       <c r="L75">
-        <v>2.1909999999999998</v>
+        <v>7.2430000000000003</v>
       </c>
       <c r="M75">
-        <v>-6.7789999999999999</v>
+        <v>7.6749999999999998</v>
       </c>
       <c r="N75">
         <v>140.191</v>
@@ -6646,10 +6646,10 @@
         <v>6.2949999999999999</v>
       </c>
       <c r="U75">
-        <v>0.121</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="V75">
-        <v>-0.19900000000000001</v>
+        <v>2E-3</v>
       </c>
       <c r="W75">
         <v>14.2</v>
@@ -6696,10 +6696,10 @@
         <v>14.735599999999998</v>
       </c>
       <c r="L76">
-        <v>0.878</v>
+        <v>4.4489999999999998</v>
       </c>
       <c r="M76">
-        <v>-7.851</v>
+        <v>5.157</v>
       </c>
       <c r="N76">
         <v>133.042</v>
@@ -6723,10 +6723,10 @@
         <v>8.2040000000000006</v>
       </c>
       <c r="U76">
-        <v>-0.19600000000000001</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="V76">
-        <v>-0.155</v>
+        <v>0.14799999999999999</v>
       </c>
       <c r="W76">
         <v>24.733000000000001</v>
@@ -6773,10 +6773,10 @@
         <v>14.7239</v>
       </c>
       <c r="L77">
-        <v>-1.758</v>
+        <v>3.9470000000000001</v>
       </c>
       <c r="M77">
-        <v>-7.6219999999999999</v>
+        <v>5.5789999999999997</v>
       </c>
       <c r="N77">
         <v>125.54</v>
@@ -6800,10 +6800,10 @@
         <v>5.7329999999999997</v>
       </c>
       <c r="U77">
-        <v>-0.161</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="V77">
-        <v>-0.218</v>
+        <v>-2.5999999999999999E-2</v>
       </c>
       <c r="W77">
         <v>20.23</v>
@@ -6850,10 +6850,10 @@
         <v>14.7036</v>
       </c>
       <c r="L78">
-        <v>-2.1059999999999999</v>
+        <v>4.242</v>
       </c>
       <c r="M78">
-        <v>-10.909000000000001</v>
+        <v>4.524</v>
       </c>
       <c r="N78">
         <v>103.676</v>
@@ -6877,10 +6877,10 @@
         <v>6.2930000000000001</v>
       </c>
       <c r="U78">
-        <v>-0.13700000000000001</v>
+        <v>1.2999999999999999E-2</v>
       </c>
       <c r="V78">
-        <v>-3.4000000000000002E-2</v>
+        <v>0.08</v>
       </c>
       <c r="W78">
         <v>20.992000000000001</v>
@@ -6927,10 +6927,10 @@
         <v>14.698600000000001</v>
       </c>
       <c r="L79">
-        <v>-2.5579999999999998</v>
+        <v>4.5209999999999999</v>
       </c>
       <c r="M79">
-        <v>-7.7050000000000001</v>
+        <v>9.6980000000000004</v>
       </c>
       <c r="N79">
         <v>82.897999999999996</v>
@@ -6954,10 +6954,10 @@
         <v>5.202</v>
       </c>
       <c r="U79">
-        <v>4.2000000000000003E-2</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="V79">
-        <v>-8.8999999999999996E-2</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="W79">
         <v>12.787000000000001</v>
@@ -7004,10 +7004,10 @@
         <v>14.8279</v>
       </c>
       <c r="L80">
-        <v>-6.9560000000000004</v>
+        <v>1.121</v>
       </c>
       <c r="M80">
-        <v>-14.231999999999999</v>
+        <v>2.891</v>
       </c>
       <c r="N80">
         <v>55.359000000000002</v>
@@ -7031,10 +7031,10 @@
         <v>6.9160000000000004</v>
       </c>
       <c r="U80">
-        <v>0.13300000000000001</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="V80">
-        <v>-0.13900000000000001</v>
+        <v>-0.16400000000000001</v>
       </c>
       <c r="W80">
         <v>9.5180000000000007</v>
@@ -7081,10 +7081,10 @@
         <v>14.791700000000002</v>
       </c>
       <c r="L81">
-        <v>-12.254</v>
+        <v>0.63800000000000001</v>
       </c>
       <c r="M81">
-        <v>-20.792000000000002</v>
+        <v>2.9039999999999999</v>
       </c>
       <c r="N81">
         <v>37.591000000000001</v>
@@ -7108,10 +7108,10 @@
         <v>6.5839999999999996</v>
       </c>
       <c r="U81">
-        <v>-8.3000000000000004E-2</v>
+        <v>0.17299999999999999</v>
       </c>
       <c r="V81">
-        <v>-0.06</v>
+        <v>8.6999999999999994E-2</v>
       </c>
       <c r="W81">
         <v>6.5620000000000003</v>
@@ -7158,10 +7158,10 @@
         <v>14.940999999999999</v>
       </c>
       <c r="L82">
-        <v>-12.430999999999999</v>
+        <v>0.52500000000000002</v>
       </c>
       <c r="M82">
-        <v>-21.736999999999998</v>
+        <v>2.3980000000000001</v>
       </c>
       <c r="N82">
         <v>25.870999999999999</v>
@@ -7185,10 +7185,10 @@
         <v>9.3529999999999998</v>
       </c>
       <c r="U82">
-        <v>0.20300000000000001</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="V82">
-        <v>-7.0999999999999994E-2</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="W82">
         <v>7.5819999999999999</v>
@@ -7235,10 +7235,10 @@
         <v>14.8764</v>
       </c>
       <c r="L83">
-        <v>-12.595000000000001</v>
+        <v>0.36699999999999999</v>
       </c>
       <c r="M83">
-        <v>-22.808</v>
+        <v>1.411</v>
       </c>
       <c r="N83">
         <v>18.632999999999999</v>
@@ -7262,10 +7262,10 @@
         <v>10.214</v>
       </c>
       <c r="U83">
-        <v>5.0000000000000001E-3</v>
+        <v>0.04</v>
       </c>
       <c r="V83">
-        <v>0.29699999999999999</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="W83">
         <v>6.6210000000000004</v>
@@ -7312,10 +7312,10 @@
         <v>14.779399999999999</v>
       </c>
       <c r="L84">
-        <v>-12.423</v>
+        <v>0.35899999999999999</v>
       </c>
       <c r="M84">
-        <v>-24.512</v>
+        <v>0.56399999999999995</v>
       </c>
       <c r="N84">
         <v>19.119</v>
@@ -7339,10 +7339,10 @@
         <v>9.9179999999999993</v>
       </c>
       <c r="U84">
-        <v>0.161</v>
+        <v>0.17199999999999999</v>
       </c>
       <c r="V84">
-        <v>0.184</v>
+        <v>0.09</v>
       </c>
       <c r="W84">
         <v>6.7220000000000004</v>
@@ -7389,10 +7389,10 @@
         <v>14.932699999999999</v>
       </c>
       <c r="L85">
-        <v>-12.545</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="M85">
-        <v>-23.678999999999998</v>
+        <v>0.65400000000000003</v>
       </c>
       <c r="N85">
         <v>13.026999999999999</v>
@@ -7416,10 +7416,10 @@
         <v>10.097</v>
       </c>
       <c r="U85">
-        <v>-0.04</v>
+        <v>0.13200000000000001</v>
       </c>
       <c r="V85">
-        <v>-0.27800000000000002</v>
+        <v>0.11700000000000001</v>
       </c>
       <c r="W85">
         <v>5.9690000000000003</v>
@@ -7466,10 +7466,10 @@
         <v>14.744199999999999</v>
       </c>
       <c r="L86">
-        <v>-12.881</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="M86">
-        <v>-25.021999999999998</v>
+        <v>0.48199999999999998</v>
       </c>
       <c r="N86">
         <v>7.7770000000000001</v>
@@ -7493,10 +7493,10 @@
         <v>12.906000000000001</v>
       </c>
       <c r="U86">
-        <v>6.4000000000000001E-2</v>
+        <v>0.309</v>
       </c>
       <c r="V86">
-        <v>-0.03</v>
+        <v>0.505</v>
       </c>
       <c r="W86">
         <v>5.008</v>
@@ -7543,10 +7543,10 @@
         <v>14.897300000000001</v>
       </c>
       <c r="L87">
-        <v>-12.901999999999999</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="M87">
-        <v>-25.603000000000002</v>
+        <v>9.4E-2</v>
       </c>
       <c r="N87">
         <v>10.603999999999999</v>
@@ -7570,10 +7570,10 @@
         <v>15.199</v>
       </c>
       <c r="U87">
-        <v>7.0000000000000001E-3</v>
+        <v>0.433</v>
       </c>
       <c r="V87">
-        <v>4.4999999999999998E-2</v>
+        <v>0.308</v>
       </c>
       <c r="W87">
         <v>5.5679999999999996</v>
@@ -7620,10 +7620,10 @@
         <v>14.927899999999998</v>
       </c>
       <c r="L88">
-        <v>-12.919</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="M88">
-        <v>-25.073</v>
+        <v>0.28799999999999998</v>
       </c>
       <c r="N88">
         <v>5.9749999999999996</v>
@@ -7647,10 +7647,10 @@
         <v>17.388000000000002</v>
       </c>
       <c r="U88">
-        <v>0.22800000000000001</v>
+        <v>0.49299999999999999</v>
       </c>
       <c r="V88">
-        <v>6.5000000000000002E-2</v>
+        <v>0.497</v>
       </c>
       <c r="W88">
         <v>6.665</v>
@@ -7697,10 +7697,10 @@
         <v>15.055599999999998</v>
       </c>
       <c r="L89">
-        <v>-12.964</v>
+        <v>-0.01</v>
       </c>
       <c r="M89">
-        <v>-25.814</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="N89">
         <v>6.53</v>
@@ -7724,10 +7724,10 @@
         <v>20.492999999999999</v>
       </c>
       <c r="U89">
-        <v>0.39200000000000002</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="V89">
-        <v>2.3E-2</v>
+        <v>0.59799999999999998</v>
       </c>
       <c r="W89">
         <v>7.234</v>
@@ -7774,10 +7774,10 @@
         <v>14.839299999999998</v>
       </c>
       <c r="L90">
-        <v>-13.038</v>
+        <v>-0.01</v>
       </c>
       <c r="M90">
-        <v>-25.907</v>
+        <v>2.7E-2</v>
       </c>
       <c r="N90">
         <v>2.9129999999999998</v>
@@ -7801,10 +7801,10 @@
         <v>15.757999999999999</v>
       </c>
       <c r="U90">
-        <v>0.496</v>
+        <v>0.47699999999999998</v>
       </c>
       <c r="V90">
-        <v>9.6000000000000002E-2</v>
+        <v>0.44900000000000001</v>
       </c>
       <c r="W90">
         <v>6.02</v>
@@ -7851,10 +7851,10 @@
         <v>15.0076</v>
       </c>
       <c r="L91">
-        <v>-13.031000000000001</v>
+        <v>-1.9E-2</v>
       </c>
       <c r="M91">
-        <v>-25.956</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="N91">
         <v>2.2799999999999998</v>
@@ -7878,10 +7878,10 @@
         <v>20.922000000000001</v>
       </c>
       <c r="U91">
-        <v>0.216</v>
+        <v>0.56200000000000006</v>
       </c>
       <c r="V91">
-        <v>0.438</v>
+        <v>0.67500000000000004</v>
       </c>
       <c r="W91">
         <v>6.6639999999999997</v>
@@ -7928,10 +7928,10 @@
         <v>14.798400000000001</v>
       </c>
       <c r="L92">
-        <v>-12.951000000000001</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="M92">
-        <v>-25.939</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="N92">
         <v>3.4220000000000002</v>
@@ -7955,10 +7955,10 @@
         <v>15.794</v>
       </c>
       <c r="U92">
-        <v>0.126</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="V92">
-        <v>-0.18</v>
+        <v>0.64800000000000002</v>
       </c>
       <c r="W92">
         <v>4.9160000000000004</v>
@@ -8005,10 +8005,10 @@
         <v>15.038699999999999</v>
       </c>
       <c r="L93">
-        <v>-12.967000000000001</v>
+        <v>-1.6E-2</v>
       </c>
       <c r="M93">
-        <v>-25.837</v>
+        <v>9.2999999999999999E-2</v>
       </c>
       <c r="N93">
         <v>3.379</v>
@@ -8032,10 +8032,10 @@
         <v>17.827000000000002</v>
       </c>
       <c r="U93">
-        <v>-9.0999999999999998E-2</v>
+        <v>0.38</v>
       </c>
       <c r="V93">
-        <v>0.13400000000000001</v>
+        <v>0.34100000000000003</v>
       </c>
       <c r="W93">
         <v>6.0259999999999998</v>
@@ -8082,10 +8082,10 @@
         <v>14.9117</v>
       </c>
       <c r="L94">
-        <v>-12.952999999999999</v>
+        <v>1.9E-2</v>
       </c>
       <c r="M94">
-        <v>-25.815000000000001</v>
+        <v>4.7E-2</v>
       </c>
       <c r="N94">
         <v>2.3620000000000001</v>
@@ -8109,10 +8109,10 @@
         <v>17.605</v>
       </c>
       <c r="U94">
-        <v>0.124</v>
+        <v>0.73099999999999998</v>
       </c>
       <c r="V94">
-        <v>7.6999999999999999E-2</v>
+        <v>0.71399999999999997</v>
       </c>
       <c r="W94">
         <v>5.4790000000000001</v>
@@ -8159,10 +8159,10 @@
         <v>14.9832</v>
       </c>
       <c r="L95">
-        <v>-12.958</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="M95">
-        <v>-25.6</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="N95">
         <v>3.1850000000000001</v>
@@ -8186,10 +8186,10 @@
         <v>17.994</v>
       </c>
       <c r="U95">
-        <v>0.25900000000000001</v>
+        <v>0.63500000000000001</v>
       </c>
       <c r="V95">
-        <v>-6.8000000000000005E-2</v>
+        <v>0.51</v>
       </c>
       <c r="W95">
         <v>5.9050000000000002</v>
@@ -8236,10 +8236,10 @@
         <v>15.120800000000001</v>
       </c>
       <c r="L96">
-        <v>41.268999999999998</v>
+        <v>46.628999999999998</v>
       </c>
       <c r="M96">
-        <v>42.341999999999999</v>
+        <v>58.061999999999998</v>
       </c>
       <c r="N96">
         <v>137.90799999999999</v>
@@ -8263,10 +8263,10 @@
         <v>10.631</v>
       </c>
       <c r="U96">
-        <v>-5.6000000000000001E-2</v>
+        <v>1.9E-2</v>
       </c>
       <c r="V96">
-        <v>-0.12</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="W96">
         <v>22.516999999999999</v>
@@ -8313,10 +8313,10 @@
         <v>14.8485</v>
       </c>
       <c r="L97">
-        <v>26.25</v>
+        <v>32.131</v>
       </c>
       <c r="M97">
-        <v>31.733000000000001</v>
+        <v>45.954000000000001</v>
       </c>
       <c r="N97">
         <v>163.17099999999999</v>
@@ -8340,10 +8340,10 @@
         <v>10.587999999999999</v>
       </c>
       <c r="U97">
-        <v>0.17499999999999999</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="V97">
-        <v>-0.22700000000000001</v>
+        <v>5.6000000000000001E-2</v>
       </c>
       <c r="W97">
         <v>25.95</v>
@@ -8390,10 +8390,10 @@
         <v>14.8687</v>
       </c>
       <c r="L98">
-        <v>14.595000000000001</v>
+        <v>19.393000000000001</v>
       </c>
       <c r="M98">
-        <v>26.95</v>
+        <v>41.095999999999997</v>
       </c>
       <c r="N98">
         <v>95.091999999999999</v>
@@ -8417,10 +8417,10 @@
         <v>8.8219999999999992</v>
       </c>
       <c r="U98">
-        <v>6.2E-2</v>
+        <v>-4.2999999999999997E-2</v>
       </c>
       <c r="V98">
-        <v>0.309</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="W98">
         <v>12.606999999999999</v>
@@ -8467,10 +8467,10 @@
         <v>14.982800000000001</v>
       </c>
       <c r="L99">
-        <v>2.335</v>
+        <v>7.7590000000000003</v>
       </c>
       <c r="M99">
-        <v>-5.1980000000000004</v>
+        <v>12.361000000000001</v>
       </c>
       <c r="N99">
         <v>57.457999999999998</v>
@@ -8494,10 +8494,10 @@
         <v>9.7970000000000006</v>
       </c>
       <c r="U99">
-        <v>-0.09</v>
+        <v>0.217</v>
       </c>
       <c r="V99">
-        <v>0.23799999999999999</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="W99">
         <v>8.6</v>
@@ -8544,10 +8544,10 @@
         <v>14.965300000000001</v>
       </c>
       <c r="L100">
-        <v>-9.5449999999999999</v>
+        <v>1.911</v>
       </c>
       <c r="M100">
-        <v>-17.36</v>
+        <v>4.5259999999999998</v>
       </c>
       <c r="N100">
         <v>23.402000000000001</v>
@@ -8571,10 +8571,10 @@
         <v>10.513</v>
       </c>
       <c r="U100">
-        <v>9.1999999999999998E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="V100">
-        <v>-0.26800000000000002</v>
+        <v>0</v>
       </c>
       <c r="W100">
         <v>5.3230000000000004</v>
@@ -8621,10 +8621,10 @@
         <v>15.2561</v>
       </c>
       <c r="L101">
-        <v>-13</v>
+        <v>-0.02</v>
       </c>
       <c r="M101">
-        <v>-25.896999999999998</v>
+        <v>-7.0000000000000001E-3</v>
       </c>
       <c r="N101">
         <v>1.8560000000000001</v>
@@ -8648,10 +8648,10 @@
         <v>17.959</v>
       </c>
       <c r="U101">
-        <v>0.95</v>
+        <v>0.77600000000000002</v>
       </c>
       <c r="V101">
-        <v>0.92700000000000005</v>
+        <v>1.014</v>
       </c>
       <c r="W101">
         <v>6.3410000000000002</v>
@@ -8698,10 +8698,10 @@
         <v>15.081700000000001</v>
       </c>
       <c r="L102">
-        <v>-9.9250000000000007</v>
+        <v>1.8420000000000001</v>
       </c>
       <c r="M102">
-        <v>-16.640999999999998</v>
+        <v>5.1849999999999996</v>
       </c>
       <c r="N102">
         <v>15.144</v>
@@ -8725,10 +8725,10 @@
         <v>10.393000000000001</v>
       </c>
       <c r="U102">
-        <v>0.11799999999999999</v>
+        <v>4.7E-2</v>
       </c>
       <c r="V102">
-        <v>0.38700000000000001</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="W102">
         <v>5.0030000000000001</v>
@@ -8775,10 +8775,10 @@
         <v>15.1807</v>
       </c>
       <c r="L103">
-        <v>-6.1680000000000001</v>
+        <v>4.4610000000000003</v>
       </c>
       <c r="M103">
-        <v>-16.164000000000001</v>
+        <v>5.0179999999999998</v>
       </c>
       <c r="N103">
         <v>23.449000000000002</v>
@@ -8802,10 +8802,10 @@
         <v>10.827</v>
       </c>
       <c r="U103">
-        <v>0.15</v>
+        <v>-1.6E-2</v>
       </c>
       <c r="V103">
-        <v>0.159</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="W103">
         <v>7.1719999999999997</v>
@@ -8852,10 +8852,10 @@
         <v>15.2082</v>
       </c>
       <c r="L104">
-        <v>-8.5039999999999996</v>
+        <v>2.2160000000000002</v>
       </c>
       <c r="M104">
-        <v>-20.626999999999999</v>
+        <v>2.9990000000000001</v>
       </c>
       <c r="N104">
         <v>23.797000000000001</v>
@@ -8879,10 +8879,10 @@
         <v>10.715999999999999</v>
       </c>
       <c r="U104">
-        <v>-0.122</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="V104">
-        <v>-2.8000000000000001E-2</v>
+        <v>3.1E-2</v>
       </c>
       <c r="W104">
         <v>5.5</v>
@@ -8929,10 +8929,10 @@
         <v>14.9954</v>
       </c>
       <c r="L105">
-        <v>-9.2680000000000007</v>
+        <v>2.1779999999999999</v>
       </c>
       <c r="M105">
-        <v>-19.815999999999999</v>
+        <v>2.2650000000000001</v>
       </c>
       <c r="N105">
         <v>15.183999999999999</v>
@@ -8956,10 +8956,10 @@
         <v>9.9309999999999992</v>
       </c>
       <c r="U105">
-        <v>0.10100000000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="V105">
-        <v>-2E-3</v>
+        <v>0.16</v>
       </c>
       <c r="W105">
         <v>4.4390000000000001</v>
@@ -9006,10 +9006,10 @@
         <v>15.008199999999999</v>
       </c>
       <c r="L106">
-        <v>-12.263999999999999</v>
+        <v>0.27700000000000002</v>
       </c>
       <c r="M106">
-        <v>-23.349</v>
+        <v>0.98699999999999999</v>
       </c>
       <c r="N106">
         <v>11.755000000000001</v>
@@ -9033,10 +9033,10 @@
         <v>9.7929999999999993</v>
       </c>
       <c r="U106">
-        <v>-5.0999999999999997E-2</v>
+        <v>0.13</v>
       </c>
       <c r="V106">
-        <v>0.10100000000000001</v>
+        <v>0.183</v>
       </c>
       <c r="W106">
         <v>3.7290000000000001</v>
@@ -9083,10 +9083,10 @@
         <v>14.808</v>
       </c>
       <c r="L107">
-        <v>-12.69</v>
+        <v>0.159</v>
       </c>
       <c r="M107">
-        <v>-24.632000000000001</v>
+        <v>0.59</v>
       </c>
       <c r="N107">
         <v>9.8070000000000004</v>
@@ -9110,10 +9110,10 @@
         <v>10.875</v>
       </c>
       <c r="U107">
-        <v>0.51300000000000001</v>
+        <v>0.73</v>
       </c>
       <c r="V107">
-        <v>0.59399999999999997</v>
+        <v>0.54100000000000004</v>
       </c>
       <c r="W107">
         <v>8.4930000000000003</v>
@@ -9160,10 +9160,10 @@
         <v>14.736599999999999</v>
       </c>
       <c r="L108">
-        <v>-12.683999999999999</v>
+        <v>0.122</v>
       </c>
       <c r="M108">
-        <v>-25.047999999999998</v>
+        <v>0.34</v>
       </c>
       <c r="N108">
         <v>6.8659999999999997</v>
@@ -9187,10 +9187,10 @@
         <v>11.257999999999999</v>
       </c>
       <c r="U108">
-        <v>0.51400000000000001</v>
+        <v>0.58599999999999997</v>
       </c>
       <c r="V108">
-        <v>0.36099999999999999</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="W108">
         <v>7.8129999999999997</v>
@@ -9237,10 +9237,10 @@
         <v>14.873100000000001</v>
       </c>
       <c r="L109">
-        <v>-12.708</v>
+        <v>0.125</v>
       </c>
       <c r="M109">
-        <v>-25.588000000000001</v>
+        <v>0.17</v>
       </c>
       <c r="N109">
         <v>11.323</v>
@@ -9264,10 +9264,10 @@
         <v>12.785</v>
       </c>
       <c r="U109">
-        <v>0.78400000000000003</v>
+        <v>0.93899999999999995</v>
       </c>
       <c r="V109">
-        <v>0.91700000000000004</v>
+        <v>1.2609999999999999</v>
       </c>
       <c r="W109">
         <v>9.3859999999999992</v>
@@ -9314,10 +9314,10 @@
         <v>14.8888</v>
       </c>
       <c r="L110">
-        <v>-12.759</v>
+        <v>9.6000000000000002E-2</v>
       </c>
       <c r="M110">
-        <v>-25.408999999999999</v>
+        <v>0.155</v>
       </c>
       <c r="N110">
         <v>8.0009999999999994</v>
@@ -9341,10 +9341,10 @@
         <v>14.734</v>
       </c>
       <c r="U110">
-        <v>0.95299999999999996</v>
+        <v>0.89600000000000002</v>
       </c>
       <c r="V110">
-        <v>0.91900000000000004</v>
+        <v>1.244</v>
       </c>
       <c r="W110">
         <v>9.6359999999999992</v>
@@ -9391,10 +9391,10 @@
         <v>14.7347</v>
       </c>
       <c r="L111">
-        <v>-12.789</v>
+        <v>0.122</v>
       </c>
       <c r="M111">
-        <v>-25.353000000000002</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="N111">
         <v>3.97</v>
@@ -9418,10 +9418,10 @@
         <v>12.782999999999999</v>
       </c>
       <c r="U111">
-        <v>0.96599999999999997</v>
+        <v>0.91100000000000003</v>
       </c>
       <c r="V111">
-        <v>1.419</v>
+        <v>1.294</v>
       </c>
       <c r="W111">
         <v>7.4450000000000003</v>
@@ -9468,10 +9468,10 @@
         <v>14.929000000000002</v>
       </c>
       <c r="L112">
-        <v>-12.648999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="M112">
-        <v>-25.353000000000002</v>
+        <v>0.124</v>
       </c>
       <c r="N112">
         <v>5.6219999999999999</v>
@@ -9495,10 +9495,10 @@
         <v>15.13</v>
       </c>
       <c r="U112">
-        <v>0.755</v>
+        <v>0.81100000000000005</v>
       </c>
       <c r="V112">
-        <v>0.80100000000000005</v>
+        <v>0.93</v>
       </c>
       <c r="W112">
         <v>8.2829999999999995</v>
@@ -9545,10 +9545,10 @@
         <v>14.8643</v>
       </c>
       <c r="L113">
-        <v>-12.82</v>
+        <v>0.107</v>
       </c>
       <c r="M113">
-        <v>-25.606999999999999</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="N113">
         <v>4.91</v>
@@ -9572,10 +9572,10 @@
         <v>14.21</v>
       </c>
       <c r="U113">
-        <v>0.76800000000000002</v>
+        <v>0.95599999999999996</v>
       </c>
       <c r="V113">
-        <v>0.95799999999999996</v>
+        <v>1.1659999999999999</v>
       </c>
       <c r="W113">
         <v>7.7190000000000003</v>
@@ -9622,10 +9622,10 @@
         <v>14.8782</v>
       </c>
       <c r="L114">
-        <v>-12.884</v>
+        <v>6.3E-2</v>
       </c>
       <c r="M114">
-        <v>-25.507000000000001</v>
+        <v>0.19800000000000001</v>
       </c>
       <c r="N114">
         <v>4.931</v>
@@ -9649,10 +9649,10 @@
         <v>14.19</v>
       </c>
       <c r="U114">
-        <v>0.878</v>
+        <v>0.91800000000000004</v>
       </c>
       <c r="V114">
-        <v>0.97399999999999998</v>
+        <v>1.0580000000000001</v>
       </c>
       <c r="W114">
         <v>7.6660000000000004</v>
@@ -9699,10 +9699,10 @@
         <v>14.773</v>
       </c>
       <c r="L115">
-        <v>-12.862</v>
+        <v>7.4999999999999997E-2</v>
       </c>
       <c r="M115">
-        <v>-25.72</v>
+        <v>0.13100000000000001</v>
       </c>
       <c r="N115">
         <v>7.3280000000000003</v>
@@ -9726,10 +9726,10 @@
         <v>14.199</v>
       </c>
       <c r="U115">
-        <v>0.78400000000000003</v>
+        <v>1.08</v>
       </c>
       <c r="V115">
-        <v>1.4370000000000001</v>
+        <v>1.57</v>
       </c>
       <c r="W115">
         <v>7.52</v>
@@ -9776,10 +9776,10 @@
         <v>14.7494</v>
       </c>
       <c r="L116">
-        <v>-12.847</v>
+        <v>0.108</v>
       </c>
       <c r="M116">
-        <v>-25.553999999999998</v>
+        <v>0.11899999999999999</v>
       </c>
       <c r="N116">
         <v>5.8680000000000003</v>
@@ -9803,10 +9803,10 @@
         <v>12.920999999999999</v>
       </c>
       <c r="U116">
-        <v>0.79800000000000004</v>
+        <v>0.93700000000000006</v>
       </c>
       <c r="V116">
-        <v>0.86699999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="W116">
         <v>6.867</v>
@@ -9853,10 +9853,10 @@
         <v>13.927299999999999</v>
       </c>
       <c r="L117">
-        <v>-12.997999999999999</v>
+        <v>-0.05</v>
       </c>
       <c r="M117">
-        <v>-26.047999999999998</v>
+        <v>-3.4000000000000002E-2</v>
       </c>
       <c r="N117">
         <v>0.112</v>
@@ -9871,10 +9871,10 @@
         <v>0.18099999999999999</v>
       </c>
       <c r="U117">
-        <v>0.01</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="V117">
-        <v>-0.161</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="W117">
         <v>0.106</v>
@@ -9921,10 +9921,10 @@
         <v>14.003699999999998</v>
       </c>
       <c r="L118">
-        <v>-13.055999999999999</v>
+        <v>-0.05</v>
       </c>
       <c r="M118">
-        <v>-26.021999999999998</v>
+        <v>-6.2E-2</v>
       </c>
       <c r="N118">
         <v>9.4E-2</v>
@@ -9939,10 +9939,10 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="U118">
-        <v>-6.2E-2</v>
+        <v>-1.4E-2</v>
       </c>
       <c r="V118">
-        <v>-0.186</v>
+        <v>-2.4E-2</v>
       </c>
       <c r="W118">
         <v>-5.5E-2</v>

</xml_diff>